<commit_message>
end to end run, all worked.
</commit_message>
<xml_diff>
--- a/daftar_berita/cnbc.xlsx
+++ b/daftar_berita/cnbc.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,12 +463,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Avanza Tersingkir Lagi, Mobil Ini Makin Sah Jadi Raja Jalanan RINews12 menit yang lalu</t>
+          <t>Asing Bawa Kabur Rp 42 T, Risiko Gagal Bayar RI Naik DrastisResearch5 menit yang lalu</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -478,7 +478,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250927215440-4-670763/avanza-tersingkir-lagi-mobil-ini-makin-sah-jadi-raja-jalanan-ri</t>
+          <t>https://www.cnbcindonesia.com/research/20250929081207-128-670925/asing-bawa-kabur-rp-42-t-risiko-gagal-bayar-ri-naik-drastis</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -486,12 +486,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Lengkap! Ini Perintah Prabowo Buntut Kasus Keracunan MBGNews20 menit yang lalu</t>
+          <t>Daftar Bunga Deposito Rupiah &amp; Dolar BRI, BNI-Mandiri per 29 SeptemberResearch10 menit yang lalu</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -501,7 +501,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250928161611-4-670845/lengkap-ini-perintah-prabowo-buntut-kasus-keracunan-mbg</t>
+          <t>https://www.cnbcindonesia.com/research/20250929053349-128-670903/daftar-bunga-deposito-rupiah-dolar-bri-bni-mandiri-per-29-september</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -509,12 +509,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Anindya Bakrie Buka Suara Soal Kuasai Tol Cibitung-CilincingMarket27 menit yang lalu</t>
+          <t>Sepatu Impor Serang Pasar Senen dan Jatinegara, Mereknya Bikin KagetNews10 menit yang lalu</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -524,7 +524,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250927212653-17-670758/anindya-bakrie-buka-suara-soal-kuasai-tol-cibitung-cilincing</t>
+          <t>https://www.cnbcindonesia.com/news/20250928200659-4-670881/sepatu-impor-serang-pasar-senen-dan-jatinegara-mereknya-bikin-kaget</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -532,12 +532,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Buntut Keracunan MBG, Pemerintah Wajibkan SPPG Punya SLHSNews29 menit yang lalu</t>
+          <t>Rekor Lagi! Harga Emas Antam Logam Mulia Hari Ini Hampir Rp 2,2 JutaResearch15 menit yang lalu</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -547,24 +547,20 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250928160936-4-670844/buntut-keracunan-mbg-pemerintah-wajibkan-sppg-punya-slhs</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>mbg</t>
-        </is>
-      </c>
+          <t>https://www.cnbcindonesia.com/research/20250929083802-128-670932/rekor-lagi-harga-emas-antam-logam-mulia-hari-ini-hampir-rp-22-juta</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Tok! Proyek Tol Terpanjang di RI Akhirnya Dipotong, Cuma Sampai SiniNews42 menit yang lalu</t>
+          <t>Bank Syariah Nasional Resmi Dapat Izin Operasi dari OJKMarket19 menit yang lalu</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -574,7 +570,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250927211640-4-670754/tok-proyek-tol-terpanjang-di-ri-akhirnya-dipotong-cuma-sampai-sini</t>
+          <t>https://www.cnbcindonesia.com/market/20250929090720-17-670950/bank-syariah-nasional-resmi-dapat-izin-operasi-dari-ojk</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -582,12 +578,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CNBC InsightSudah Jelas Korupsi, Pejabat di Jakarta Malah Dikasih Kenaikan JabatanEntrepreneur57 menit yang lalu</t>
+          <t>IHSG Dibuka Menguat, Balik Lagi ke Level 8.100Market25 menit yang lalu</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -597,7 +593,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/entrepreneur/20250908093807-25-664908/sudah-jelas-korupsi-pejabat-di-jakarta-malah-dikasih-kenaikan-jabatan</t>
+          <t>https://www.cnbcindonesia.com/market/20250929084220-17-670933/ihsg-dibuka-menguat-balik-lagi-ke-level-8100</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -605,12 +601,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Prabowo Perintahkan SPPG Bermasalah Ditutup Usai Kasus Keracunan MBGNews1 jam yang lalu</t>
+          <t>Pemerintah Tetapkan Tarif Listrik Oktober-Desember 2025, Ini DaftarnyaNews25 menit yang lalu</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -620,7 +616,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250928153901-4-670843/prabowo-perintahkan-sppg-bermasalah-ditutup-usai-kasus-keracunan-mbg</t>
+          <t>https://www.cnbcindonesia.com/news/20250929075531-4-670921/pemerintah-tetapkan-tarif-listrik-oktober-desember-2025-ini-daftarnya</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
@@ -628,12 +624,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Gelar Upacara HUT ke-80, KAI Pertegas Semangat MelayaniNews1 jam yang lalu</t>
+          <t>Breaking! Rupiah Perkasa, Dolar AS Turun ke Rp16.640Market26 menit yang lalu</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -643,7 +639,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250928152912-4-670841/gelar-upacara-hut-ke-80-kai-pertegas-semangat-melayani</t>
+          <t>https://www.cnbcindonesia.com/market/20250929082543-17-670927/breaking-rupiah-perkasa-dolar-as-turun-ke-rp16640</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -651,12 +647,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Ada Tol Baru, Jakarta-Bandung Sebentar Lagi Bisa Secepat KilatNews1 jam yang lalu</t>
+          <t>InternasionalRaja Singa Tiba-Tiba Meledak di Sini, Kasus Naik 460%News30 menit yang lalu</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -666,7 +662,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250927210415-4-670750/ada-tol-baru-jakarta-bandung-sebentar-lagi-bisa-secepat-kilat</t>
+          <t>https://www.cnbcindonesia.com/news/20250929084616-4-670934/raja-singa-tiba-tiba-meledak-di-sini-kasus-naik-460</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -674,12 +670,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Raksasa Tekstil Asal Bandung Resmi Pailit, Ini Nama PerusahaannyaMarket1 jam yang lalu</t>
+          <t>Netizen Teriak M-banking BCA &amp; blu Kompak Error, Ini Kata ManajemenMarket37 menit yang lalu</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -689,7 +685,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250927220319-17-670766/raksasa-tekstil-asal-bandung-resmi-pailit-ini-nama-perusahaannya</t>
+          <t>https://www.cnbcindonesia.com/market/20250929084732-17-670940/netizen-teriak-m-banking-bca-blu-kompak-error-ini-kata-manajemen</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -697,12 +693,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Ada Cara Gratis Langganan ChatGPT Plus 3 Bulan, Hemat JutaanTech1 jam yang lalu</t>
+          <t>Pertamina Bakal Gabung 3 Anak Usahanya, Ini Respons BahlilNews45 menit yang lalu</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -712,7 +708,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250928142114-37-670837/ada-cara-gratis-langganan-chatgpt-plus-3-bulan-hemat-jutaan</t>
+          <t>https://www.cnbcindonesia.com/news/20250929074918-4-670920/pertamina-bakal-gabung-3-anak-usahanya-ini-respons-bahlil</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -720,12 +716,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Daftar Negara Tujuan Duit Crazy Rich Dunia, Ada Tetangga IndonesiaResearch1 jam yang lalu</t>
+          <t>Investor Tunggu Data Penting Australia, Bursa Asia Dibuka VariatifMarket52 menit yang lalu</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -735,7 +731,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/research/20250928135510-128-670815/daftar-negara-tujuan-duit-crazy-rich-dunia-ada-tetangga-indonesia</t>
+          <t>https://www.cnbcindonesia.com/market/20250929082751-17-670929/investor-tunggu-data-penting-australia-bursa-asia-dibuka-variatif</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -743,12 +739,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Rusia Bombardir Kyiv Pakai Rudal &amp; Drone, Suara Tembakan MenggemaNews1 jam yang lalu</t>
+          <t>Penyebab Keracunan MBG Dibeberkan Profesor Eks Direktur WHOTech55 menit yang lalu</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -758,20 +754,24 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250928125358-4-670806/rusia-bombardir-kyiv-pakai-rudal-drone-suara-tembakan-menggema</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/tech/20250929083011-37-670928/penyebab-keracunan-mbg-dibeberkan-profesor-eks-direktur-who</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>mbg</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Proyek Bandara Bali Utara Ganti Lokasi, Ini Penjelasan KemenhubNews2 jam yang lalu</t>
+          <t>Pelabuhan Tanjung Priok Bakal Dikepung Tol, Rute Terbaru Nempel JISNews1 jam yang lalu</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -781,7 +781,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250928143433-4-670838/proyek-bandara-bali-utara-ganti-lokasi-ini-penjelasan-kemenhub</t>
+          <t>https://www.cnbcindonesia.com/news/20250928193756-4-670880/pelabuhan-tanjung-priok-bakal-dikepung-tol-rute-terbaru-nempel-jis</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
@@ -789,12 +789,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Ada 4 Bangunan Terlihat Jelas dari Luar Angkasa, Ini DaftarnyaTech2 jam yang lalu</t>
+          <t>Asing Terciduk Diam-diam Lego 10 Saham Ini Kala Cetak Net Buy JumboMarket1 jam yang lalu</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -804,7 +804,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250928140001-37-670826/ada-4-bangunan-terlihat-jelas-dari-luar-angkasa-ini-daftarnya</t>
+          <t>https://www.cnbcindonesia.com/market/20250929081104-17-670923/asing-terciduk-diam-diam-lego-10-saham-ini-kala-cetak-net-buy-jumbo</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
@@ -812,12 +812,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Bandung Terancam Gempa Besar, Tandanya Sudah Terlihat di Gunung BatuNews2 jam yang lalu</t>
+          <t>Triniti Land (TRIN) Jual Saham Anak Usaha, Ada Apa?Market1 jam yang lalu</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -827,7 +827,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250927213416-4-670760/bandung-terancam-gempa-besar-tandanya-sudah-terlihat-di-gunung-batu</t>
+          <t>https://www.cnbcindonesia.com/market/20250929082043-17-670926/triniti-land--trin--jual-saham-anak-usaha-ada-apa</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
@@ -835,12 +835,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Pengemis Terkaya Dunia, Harta Rp15 M &amp; Punya ApartemenLifestyle2 jam yang lalu</t>
+          <t>BCA Mobile Down 2 Jam Ramai di Medsos, Netizen Curhat Susah ke KantorTech1 jam yang lalu</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -850,7 +850,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/lifestyle/20250928124557-33-670804/pengemis-terkaya-dunia-harta-rp15-m-punya-apartemen</t>
+          <t>https://www.cnbcindonesia.com/tech/20250929080708-37-670924/bca-mobile-down-2-jam-ramai-di-medsos-netizen-curhat-susah-ke-kantor</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -858,12 +858,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Saat Marquez Menangis usai Pastikan Gelar Juara Dunia MotoGP 2025Lifestyle2 jam yang lalu</t>
+          <t>Catat! 5 Emiten Ini Tebar Dividen Pekan IniResearch1 jam yang lalu</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -873,7 +873,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/lifestyle/20250928134111-33-670814/saat-marquez-menangis-usai-pastikan-gelar-juara-dunia-motogp-2025</t>
+          <t>https://www.cnbcindonesia.com/research/20250929052328-128-670902/catat-5-emiten-ini-tebar-dividen-pekan-ini</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
@@ -881,12 +881,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Saldo JHT BPJS Bisa Dicairkan sebelum Resign, Begini CaranyaTech2 jam yang lalu</t>
+          <t>Pertamina Siap Pasok Kebutuhan SPBU VIVO Hingga 40 Ribu Barel BBMNews1 jam yang lalu</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -896,7 +896,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250928121441-37-670801/saldo-jht-bpjs-bisa-dicairkan-sebelum-resign-begini-caranya</t>
+          <t>https://www.cnbcindonesia.com/news/20250929074116-4-670919/pertamina-siap-pasok-kebutuhan-spbu-vivo-hingga-40-ribu-barel-bbm</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
@@ -904,12 +904,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Gokil! Emas Pegadaian Sepekan Naik 3,19%, Pemilik Kipas-Kipas DuitResearch3 jam yang lalu</t>
+          <t>InternasionalChina-Korut "Bersatu", Xi Jinping-Kim Jong Un Beri Pesan Baru ke DuniaNews1 jam yang lalu</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -919,7 +919,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/research/20250928120930-128-670800/gokil-emas-pegadaian-sepekan-naik-319-pemilik-kipas-kipas-duit</t>
+          <t>https://www.cnbcindonesia.com/news/20250929070953-4-670907/china-korut-bersatu-xi-jinping-kim-jong-un-beri-pesan-baru-ke-dunia</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
@@ -927,12 +927,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Ahli Pasang Chip di 12 Kepala Manusia, Begini EfeknyaTech3 jam yang lalu</t>
+          <t>4 Poin Penting Dibahas Purbaya &amp; Bos BI Saat Santap Bebek GorengMarket1 jam yang lalu</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -942,20 +942,24 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250928122646-37-670802/ahli-pasang-chip-di-12-kepala-manusia-begini-efeknya</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/market/20250929071811-17-670910/4-poin-penting-dibahas-purbaya-bos-bi-saat-santap-bebek-goreng</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>purbaya</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Insiden Maut Kampanye, 36 Orang Tewas &amp; 50 Orang Luka-LukaNews3 jam yang lalu</t>
+          <t>Revisi UU BUMN Akan Disahkan DPR Pekan Ini, Ini 11 Poin PentingMarket1 jam yang lalu</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -965,7 +969,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250928112919-4-670799/insiden-maut-kampanye-36-orang-tewas-50-orang-luka-luka</t>
+          <t>https://www.cnbcindonesia.com/market/20250929074512-17-670922/revisi-uu-bumn-akan-disahkan-dpr-pekan-ini-ini-11-poin-penting</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
@@ -973,12 +977,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Pengamat Bongkar Modus Negatif Menyasar ke Menteri ESDMNews3 jam yang lalu</t>
+          <t>Purbaya Bicara Soal Nasib BI di RUU P2SK, Hilang Independensi?Market1 jam yang lalu</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -988,20 +992,24 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250928124408-4-670805/pengamat-bongkar-modus-negatif-menyasar-ke-menteri-esdm</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/market/20250928234637-17-670898/purbaya-bicara-soal-nasib-bi-di-ruu-p2sk-hilang-independensi</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>purbaya</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Daftar Artefak Budaya Milik Indonesia yang Mau Dikembalikan BelandaNews3 jam yang lalu</t>
+          <t>Asing Net Buy 7,38 T Pekan Lalu, Kompak Borong 10 Saham IniMarket1 jam yang lalu</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1011,7 +1019,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250928122913-4-670803/daftar-artefak-budaya-milik-indonesia-yang-mau-dikembalikan-belanda</t>
+          <t>https://www.cnbcindonesia.com/market/20250929073515-17-670918/asing-net-buy-738-t-pekan-lalu-kompak-borong-10-saham-ini</t>
         </is>
       </c>
       <c r="E25" t="inlineStr"/>
@@ -1019,12 +1027,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Lewat Program Ini, BRI Peduli Ajak Generasi Muda Jaga Ekosistem SungaiNews4 jam yang lalu</t>
+          <t>Langit Tiba-Tiba Terang Benderang Bikin Panik, Ternyata Kelakuan ChinaTech1 jam yang lalu</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1034,7 +1042,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250928112841-4-670798/lewat-program-ini-bri-peduli-ajak-generasi-muda-jaga-ekosistem-sungai</t>
+          <t>https://www.cnbcindonesia.com/tech/20250928224447-37-670894/langit-tiba-tiba-terang-benderang-bikin-panik-ternyata-kelakuan-china</t>
         </is>
       </c>
       <c r="E26" t="inlineStr"/>
@@ -1042,12 +1050,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>10 HP Pancarkan Radiasi Paling Tinggi, Ada yang Laku Keras di RITech4 jam yang lalu</t>
+          <t>InternasionalKala Bumi Ngamuk ke Netanyahu: Demo Massal-Lempar SepatuNews1 jam yang lalu</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1057,7 +1065,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250928112307-37-670796/10-hp-pancarkan-radiasi-paling-tinggi-ada-yang-laku-keras-di-ri</t>
+          <t>https://www.cnbcindonesia.com/news/20250929073240-4-670917/kala-bumi-ngamuk-ke-netanyahu-demo-massal-lempar-sepatu</t>
         </is>
       </c>
       <c r="E27" t="inlineStr"/>
@@ -1065,12 +1073,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Cara Mudah Cek KTP Kamu Dipakai Pinjol IlegalMarket4 jam yang lalu</t>
+          <t>Fenomena Langka: China &amp; Singapura Berlomba-Lomba Akuisisi Emiten RIResearch2 jam yang lalu</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1080,7 +1088,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250928100338-17-670794/cara-mudah-cek-ktp-kamu-dipakai-pinjol-ilegal</t>
+          <t>https://www.cnbcindonesia.com/research/20250926132341-128-670474/fenomena-langka-china-singapura-berlomba-lomba-akuisisi-emiten-ri</t>
         </is>
       </c>
       <c r="E28" t="inlineStr"/>
@@ -1088,12 +1096,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Asal-Usul Fenomena Kumpul Kebo, Ternyata dari Gubernur VOCNews4 jam yang lalu</t>
+          <t>Modus Baru Penipuan Incar Karyawan Pakai OTP, Google Ungkap Cara CegahTech2 jam yang lalu</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1103,7 +1111,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250928090717-4-670788/asal-usul-fenomena-kumpul-kebo-ternyata-dari-gubernur-voc</t>
+          <t>https://www.cnbcindonesia.com/tech/20250928225023-37-670895/modus-baru-penipuan-incar-karyawan-pakai-otp-google-ungkap-cara-cegah</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
@@ -1111,12 +1119,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Nampan Makan MBG Diduga Tercemar Air Limbah, Begini KondisinyaNews4 jam yang lalu</t>
+          <t>InternasionalAS di Ujung Tanduk, Trump Warning PHK PNS Besar-besaranNews2 jam yang lalu</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1126,24 +1134,20 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250928094252-4-670792/nampan-makan-mbg-diduga-tercemar-air-limbah-begini-kondisinya</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>mbg</t>
-        </is>
-      </c>
+          <t>https://www.cnbcindonesia.com/news/20250929063500-4-670906/as-di-ujung-tanduk-trump-warning-phk-pns-besar-besaran</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Jadwal &amp; Pemain Timnas Indonesia Babak 4 Kualifikasi Piala Dunia 2026Research5 jam yang lalu</t>
+          <t>Anggito Jadi Ketua LPS, Purbaya Usul ke Prabowo Tak Tambah Wamen LagiMarket2 jam yang lalu</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1153,20 +1157,24 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/research/20250928024805-128-670770/jadwal-pemain-timnas-indonesia-babak-4-kualifikasi-piala-dunia-2026</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/market/20250928230107-17-670896/anggito-jadi-ketua-lps-purbaya-usul-ke-prabowo-tak-tambah-wamen-lagi</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>purbaya</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Menteri Transmigrasi Tebar Pesona 154 Kawasan ke Investor GlobalNews5 jam yang lalu</t>
+          <t>RI Nomor Satu Paling Parah Sedunia, Harus Belajar dari JepangTech2 jam yang lalu</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1176,7 +1184,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250928111327-4-670795/menteri-transmigrasi-tebar-pesona-154-kawasan-ke-investor-global</t>
+          <t>https://www.cnbcindonesia.com/tech/20250928223656-37-670893/ri-nomor-satu-paling-parah-sedunia-harus-belajar-dari-jepang</t>
         </is>
       </c>
       <c r="E32" t="inlineStr"/>
@@ -1184,12 +1192,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>CNBC InsightTragis! Mayat Pejabat Ini Ditinggal di Jalan, Warga Ogah GotongEntrepreneur5 jam yang lalu</t>
+          <t>InternasionalPrabowo Bertemu 'Empat Mata' Dengan Trump di Sidang PBB, Katakan IniNews2 jam yang lalu</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1199,7 +1207,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/entrepreneur/20250928093413-25-670791/tragis-mayat-pejabat-ini-ditinggal-di-jalan-warga-ogah-gotong</t>
+          <t>https://www.cnbcindonesia.com/news/20250929054354-4-670905/prabowo-bertemu-empat-mata-dengan-trump-di-sidang-pbb-katakan-ini</t>
         </is>
       </c>
       <c r="E33" t="inlineStr"/>
@@ -1207,12 +1215,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Harta Karun RI Ini Jadi Incaran Pencinta Parfum &amp; Komunitas GanjaResearch5 jam yang lalu</t>
+          <t>Harga Emas Bisa Tembus Langit Pekan Ini Tapi Ada 3 SyaratnyaResearch2 jam yang lalu</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1222,7 +1230,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/research/20250928062024-128-670775/harta-karun-ri-ini-jadi-incaran-pencinta-parfum-komunitas-ganja</t>
+          <t>https://www.cnbcindonesia.com/research/20250929051305-128-670901/harga-emas-bisa-tembus-langit-pekan-ini-tapi-ada-3-syaratnya</t>
         </is>
       </c>
       <c r="E34" t="inlineStr"/>
@@ -1230,12 +1238,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Presiden Kolombia Tantang Trump usai Dilarang Masuk AmerikaNews5 jam yang lalu</t>
+          <t>Fitur Chat WhatsApp Tanpa Nomor Telepon, Cara dan LarangannyaTech3 jam yang lalu</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1245,7 +1253,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250928092055-4-670790/presiden-kolombia-tantang-trump-usai-dilarang-masuk-amerika</t>
+          <t>https://www.cnbcindonesia.com/tech/20250928222748-37-670891/fitur-chat-whatsapp-tanpa-nomor-telepon-cara-dan-larangannya</t>
         </is>
       </c>
       <c r="E35" t="inlineStr"/>
@@ -1253,12 +1261,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Cuma 3 Orang Ini Bisa Keliling Dunia Tanpa Paspor dan VisaLifestyle6 jam yang lalu</t>
+          <t>Purbaya: Saya Koboi, Pistolnya Banyak Tapi Gak SembaranganMarket3 jam yang lalu</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1268,20 +1276,24 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/lifestyle/20250928091524-33-670789/cuma-3-orang-ini-bisa-keliling-dunia-tanpa-paspor-dan-visa</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/market/20250928223403-17-670892/purbaya-saya-koboi-pistolnya-banyak-tapi-gak-sembarangan</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>purbaya</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>10 Perusahaan Batu Bara Terbesar Dunia, Mesin Utama Listrik GlobalResearch6 jam yang lalu</t>
+          <t>InternasionalSanksi Barat Gak Mempan, Putin Garap Proyek Nuklir Rp 400 T di IranNews3 jam yang lalu</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1291,7 +1303,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/research/20250926183016-131-670606/10-perusahaan-batu-bara-terbesar-dunia-mesin-utama-listrik-global</t>
+          <t>https://www.cnbcindonesia.com/news/20250929053949-4-670904/sanksi-barat-gak-mempan-putin-garap-proyek-nuklir-rp-400-t-di-iran</t>
         </is>
       </c>
       <c r="E37" t="inlineStr"/>
@@ -1299,12 +1311,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Potret Selena Gomez Resmi Menikah dengan Benny BlancoLifestyle6 jam yang lalu</t>
+          <t>NewsletterWaspada! 7 Isu Penting Bisa Bikin IHSG &amp; Rupiah 'Keringetan' Pekan IniResearch3 jam yang lalu</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1314,7 +1326,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/lifestyle/20250928095517-33-670793/potret-selena-gomez-resmi-menikah-dengan-benny-blanco</t>
+          <t>https://www.cnbcindonesia.com/research/20250929050437-128-670900/waspada-7-isu-penting-bisa-bikin-ihsg-rupiah-keringetan-pekan-ini</t>
         </is>
       </c>
       <c r="E38" t="inlineStr"/>
@@ -1322,12 +1334,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Review SepekanHarga Perak Ngebut Sepanjang Pekan, Cetak Rekor Tertinggi 14 Tahun!Research6 jam yang lalu</t>
+          <t>InternasionalHoror Penembakan Sadis di Ibadah Minggu Gereja AS, Ada Korban TewasNews4 jam yang lalu</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1337,7 +1349,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/research/20250928015036-128-670769/harga-perak-ngebut-sepanjang-pekan-cetak-rekor-tertinggi-14-tahun</t>
+          <t>https://www.cnbcindonesia.com/news/20250929043856-4-670899/horor-penembakan-sadis-di-ibadah-minggu-gereja-as-ada-korban-tewas</t>
         </is>
       </c>
       <c r="E39" t="inlineStr"/>
@@ -1345,12 +1357,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>CNBC InsightTernyata Ini Orang Pertama yang Mengenalkan Konsep Pajak di IndonesiaNews7 jam yang lalu</t>
+          <t>Prabowo Rapat Bareng Menteri Minggu Sore, Bahas MBG hingga Stok BerasNews9 jam yang lalu</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1360,20 +1372,24 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250928061151-4-670773/ternyata-ini-orang-pertama-yang-mengenalkan-konsep-pajak-di-indonesia</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/news/20250928233141-4-670897/prabowo-rapat-bareng-menteri-minggu-sore-bahas-mbg-hingga-stok-beras</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>mbg</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Kronologi Penangkapan Bos Investree, Rugikan Masyarakat Rp27 TriliunMarket7 jam yang lalu</t>
+          <t>InternasionalDemonstrasi Berujung Maut, 39 Orang Tewas karena Berdesakan-TerinjakNews11 jam yang lalu</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1383,7 +1399,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250928085147-17-670787/kronologi-penangkapan-bos-investree-rugikan-masyarakat-rp27-triliun</t>
+          <t>https://www.cnbcindonesia.com/news/20250928190245-4-670876/demonstrasi-berujung-maut-39-orang-tewas-karena-berdesakan-terinjak</t>
         </is>
       </c>
       <c r="E41" t="inlineStr"/>
@@ -1391,12 +1407,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Jelang HUT TNI, Ini Daftar Senjata Baru yang Dibeli PrabowoResearch7 jam yang lalu</t>
+          <t>Haji Isam Punya Harta Rp 101 Triliun tapi Tak Masuk Forbes, Kok Bisa?Market11 jam yang lalu</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1406,7 +1422,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/research/20250928060342-128-670772/jelang-hut-tni-ini-daftar-senjata-baru-yang-dibeli-prabowo</t>
+          <t>https://www.cnbcindonesia.com/market/20250928193130-17-670879/haji-isam-punya-harta-rp-101-triliun-tapi-tak-masuk-forbes-kok-bisa</t>
         </is>
       </c>
       <c r="E42" t="inlineStr"/>
@@ -1414,12 +1430,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Daftar 11 Aplikasi Terkenal di RI Ini Ternyata Bikinan IsraelTech7 jam yang lalu</t>
+          <t>InternasionalMedia Malaysia Soroti Transportasi Jakarta Ungguli Kuala LumpurNews12 jam yang lalu</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1429,7 +1445,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250928063629-37-670777/daftar-11-aplikasi-terkenal-di-ri-ini-ternyata-bikinan-israel</t>
+          <t>https://www.cnbcindonesia.com/news/20250928192227-4-670878/media-malaysia-soroti-transportasi-jakarta-ungguli-kuala-lumpur</t>
         </is>
       </c>
       <c r="E43" t="inlineStr"/>
@@ -1437,12 +1453,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Singapura Mulai Ditinggalkan Crazy Rich China, Ada Apa?Market8 jam yang lalu</t>
+          <t>Marak Penipuan Pakai Modus Baru Catphishing, Ini Tips HindariTech12 jam yang lalu</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1452,7 +1468,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250928063240-17-670776/singapura-mulai-ditinggalkan-crazy-rich-china-ada-apa</t>
+          <t>https://www.cnbcindonesia.com/tech/20250928191555-37-670877/marak-penipuan-pakai-modus-baru-catphishing-ini-tips-hindari</t>
         </is>
       </c>
       <c r="E44" t="inlineStr"/>
@@ -1460,12 +1476,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>CNBC InsightKisah Raja Jawa Sebar Duit Rp20 Miliar agar Rakyat Tak KelaparanLifestyle8 jam yang lalu</t>
+          <t>Menkes Ajak Sarapan 2 Telur Rebus Bukan Nasi Uduk-Bubur, Ini AlasannyaLifestyle12 jam yang lalu</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1475,7 +1491,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/lifestyle/20250927215829-33-670764/kisah-raja-jawa-sebar-duit-rp20-miliar-agar-rakyat-tak-kelaparan</t>
+          <t>https://www.cnbcindonesia.com/lifestyle/20250928184201-33-670873/menkes-ajak-sarapan-2-telur-rebus-bukan-nasi-uduk-bubur-ini-alasannya</t>
         </is>
       </c>
       <c r="E45" t="inlineStr"/>
@@ -1483,12 +1499,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Ugal-Ugalan Bangun Bom Nuklir, Iran Kena Sanksi PBBNews8 jam yang lalu</t>
+          <t>14.341 Tiket KA Rp 80.000 Gagal Dijual, Tenang! Masih Ada Diskon 20%News12 jam yang lalu</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1498,7 +1514,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250928061904-4-670774/ugal-ugalan-bangun-bom-nuklir-iran-kena-sanksi-pbb</t>
+          <t>https://www.cnbcindonesia.com/news/20250928181323-4-670859/14341-tiket-ka-rp-80000-gagal-dijual-tenang-masih-ada-diskon-20</t>
         </is>
       </c>
       <c r="E46" t="inlineStr"/>
@@ -1506,12 +1522,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Bosch Mau PHK 13.000 Karyawan, Ternyata Ini PenyebabnyaNews8 jam yang lalu</t>
+          <t>Nabi Musa Bisa Membelah Laut Merah, Begini Penjelasan IlmiahnyaTech13 jam yang lalu</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1521,7 +1537,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250927222618-4-670768/bosch-mau-phk-13000-karyawan-ternyata-ini-penyebabnya</t>
+          <t>https://www.cnbcindonesia.com/tech/20250928175524-37-670858/nabi-musa-bisa-membelah-laut-merah-begini-penjelasan-ilmiahnya</t>
         </is>
       </c>
       <c r="E47" t="inlineStr"/>
@@ -1529,12 +1545,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>7 Alat Kesehatan Gratis Pakai BPJS Kesehatan, Termasuk KacamataLifestyle9 jam yang lalu</t>
+          <t>Lewat Inovasi, Anak Usaha InJourney Raih Penghargaan di Ajang Ini!News13 jam yang lalu</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1544,7 +1560,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/lifestyle/20250927212531-33-670757/7-alat-kesehatan-gratis-pakai-bpjs-kesehatan-termasuk-kacamata</t>
+          <t>https://www.cnbcindonesia.com/news/20250928201250-4-670882/lewat-inovasi-anak-usaha-injourney-raih-penghargaan-di-ajang-ini</t>
         </is>
       </c>
       <c r="E48" t="inlineStr"/>
@@ -1552,12 +1568,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Daftar 96 Pinjol Berizin OJK Per 2025, Jangan Asal Ambil Utang!Market9 jam yang lalu</t>
+          <t>Makanan Murah Ini Bagus Buat Ibu Hamil dan Cegah Bayi StuntingLifestyle13 jam yang lalu</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1567,7 +1583,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250927221245-17-670767/daftar-96-pinjol-berizin-ojk-per-2025-jangan-asal-ambil-utang</t>
+          <t>https://www.cnbcindonesia.com/lifestyle/20250928171845-33-670849/makanan-murah-ini-bagus-buat-ibu-hamil-dan-cegah-bayi-stunting</t>
         </is>
       </c>
       <c r="E49" t="inlineStr"/>
@@ -1575,12 +1591,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>12 Negara Umumkan Dukungan Finansial untuk Palestina, Ini DaftarnyaNews9 jam yang lalu</t>
+          <t>Rahasia Satelit Bertahan Mengorbit di Angkasa Terungkap, Ternyata IniTech13 jam yang lalu</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1590,7 +1606,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250927210919-4-670752/12-negara-umumkan-dukungan-finansial-untuk-palestina-ini-daftarnya</t>
+          <t>https://www.cnbcindonesia.com/tech/20250928165143-37-670848/rahasia-satelit-bertahan-mengorbit-di-angkasa-terungkap-ternyata-ini</t>
         </is>
       </c>
       <c r="E50" t="inlineStr"/>
@@ -1598,12 +1614,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>China Luncurkan Internet 10G Pertama di Dunia, Begini KecepatannyaTech10 jam yang lalu</t>
+          <t>Siap-Siap! Rumah Murah Bakal Dibangun di Jakarta, Ini BocorannyaNews13 jam yang lalu</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1613,10 +1629,240 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250927212305-37-670756/china-luncurkan-internet-10g-pertama-di-dunia-begini-kecepatannya</t>
+          <t>https://www.cnbcindonesia.com/news/20250928133943-4-670813/siap-siap-rumah-murah-bakal-dibangun-di-jakarta-ini-bocorannya</t>
         </is>
       </c>
       <c r="E51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Tol RI Tambah Panjang Lagi 308,7 Km Tahun Depan, Tembus Yogya &amp; KediriNews14 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/news/20250927210807-4-670751/tol-ri-tambah-panjang-lagi-3087-km-tahun-depan-tembus-yogya-kediri</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Ada 9 Fenomena Langit di Oktober, Muncul Hujan Meteor-SupermoonResearch14 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/research/20250928151602-128-670840/ada-9-fenomena-langit-di-oktober-muncul-hujan-meteor-supermoon</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Peran &amp; Tantangan BPRS dalam Mendorong Ekonomi Syariah di IndonesiaNews14 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/news/20250928185539-4-670875/peran-tantangan-bprs-dalam-mendorong-ekonomi-syariah-di-indonesia</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Jalur Kereta Api Mati Mau Dihidupkan Lagi, Ini DaftarnyaNews14 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/news/20250927214927-4-670762/jalur-kereta-api-mati-mau-dihidupkan-lagi-ini-daftarnya</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Sentimen Pekan DepanWaspada! IHSG &amp; Rupiah Rawan Bergejolak karena Kabar dari AS dan ChinaResearch14 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/research/20250928033702-128-670771/waspada-ihsg-rupiah-rawan-bergejolak-karena-kabar-dari-as-dan-china</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Ada Tol Baru, Warga BSD ke Bogor Terasa SejengkalNews15 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/news/20250927211218-4-670753/ada-tol-baru-warga-bsd-ke-bogor-terasa-sejengkal</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Megathrust Meledak, Yogya Bisa Diguncang Gempa M 8,8-Digulung TsunamiTech15 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/tech/20250928150121-37-670839/megathrust-meledak-yogya-bisa-diguncang-gempa-m-88-digulung-tsunami</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>CNBC InsightPresiden RI Tolak Sosok Ini Jadi Menteri karena Idenya Terlalu GilaEntrepreneur15 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/entrepreneur/20250927214356-25-670761/presiden-ri-tolak-sosok-ini-jadi-menteri-karena-idenya-terlalu-gila</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Proyek Tol Puncak Dilelang Tahun Depan, Begini Rencana RutenyaNews15 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/news/20250927212212-4-670755/proyek-tol-puncak-dilelang-tahun-depan-begini-rencana-rutenya</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Mobil Ini Paling Gak Laku di RI, Cuma Terjual 1 UnitNews16 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/news/20250927215850-4-670765/mobil-ini-paling-gak-laku-di-ri-cuma-terjual-1-unit</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
End to End run works ok.
</commit_message>
<xml_diff>
--- a/daftar_berita/cnbc.xlsx
+++ b/daftar_berita/cnbc.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Asing Bawa Kabur Rp 42 T, Risiko Gagal Bayar RI Naik DrastisResearch5 menit yang lalu</t>
+          <t>Prabowo Selamatkan Rp22 Triliun Duit Negara dari Tambang Timah IlegalNews1 menit yang lalu</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -478,15 +478,19 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/research/20250929081207-128-670925/asing-bawa-kabur-rp-42-t-risiko-gagal-bayar-ri-naik-drastis</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/news/20250929121348-4-671056/prabowo-selamatkan-rp22-triliun-duit-negara-dari-tambang-timah-ilegal</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>prabowo</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Daftar Bunga Deposito Rupiah &amp; Dolar BRI, BNI-Mandiri per 29 SeptemberResearch10 menit yang lalu</t>
+          <t>Ini 10 Bank Syariah Penyokong Ekonomi RakyatNews4 menit yang lalu</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -501,7 +505,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/research/20250929053349-128-670903/daftar-bunga-deposito-rupiah-dolar-bri-bni-mandiri-per-29-september</t>
+          <t>https://www.cnbcindonesia.com/news/20250929133640-4-671110/ini-10-bank-syariah-penyokong-ekonomi-rakyat</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -509,7 +513,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Sepatu Impor Serang Pasar Senen dan Jatinegara, Mereknya Bikin KagetNews10 menit yang lalu</t>
+          <t>Surge (WIFI) Kompak Divestasi Saham 3 Anak UsahaMarket6 menit yang lalu</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -524,7 +528,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250928200659-4-670881/sepatu-impor-serang-pasar-senen-dan-jatinegara-mereknya-bikin-kaget</t>
+          <t>https://www.cnbcindonesia.com/market/20250929083947-17-670931/surge--wifi--kompak-divestasi-saham-3-anak-usaha</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -532,7 +536,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Rekor Lagi! Harga Emas Antam Logam Mulia Hari Ini Hampir Rp 2,2 JutaResearch15 menit yang lalu</t>
+          <t>Pelajaran Pahit China &amp; India: MBG di RI Bisa Meledak Jadi Tragedi?Research11 menit yang lalu</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -547,15 +551,19 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/research/20250929083802-128-670932/rekor-lagi-harga-emas-antam-logam-mulia-hari-ini-hampir-rp-22-juta</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/research/20250929105903-128-670999/pelajaran-pahit-china-india-mbg-di-ri-bisa-meledak-jadi-tragedi</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>mbg</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Bank Syariah Nasional Resmi Dapat Izin Operasi dari OJKMarket19 menit yang lalu</t>
+          <t>Pegadaian dan Masjid Salman ITB Daur Ulang Air Hujan dan Air WudhuNews14 menit yang lalu</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -570,7 +578,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250929090720-17-670950/bank-syariah-nasional-resmi-dapat-izin-operasi-dari-ojk</t>
+          <t>https://www.cnbcindonesia.com/news/20250929132227-4-671094/pegadaian-dan-masjid-salman-itb-daur-ulang-air-hujan-dan-air-wudhu</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -578,7 +586,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>IHSG Dibuka Menguat, Balik Lagi ke Level 8.100Market25 menit yang lalu</t>
+          <t>InternasionalTrump Mendadak Kirim Pasukan-Serbu Negara Bagian Ini, Pentagon KagetNews16 menit yang lalu</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -593,7 +601,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250929084220-17-670933/ihsg-dibuka-menguat-balik-lagi-ke-level-8100</t>
+          <t>https://www.cnbcindonesia.com/news/20250929112109-4-671019/trump-mendadak-kirim-pasukan-serbu-negara-bagian-ini-pentagon-kaget</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -601,7 +609,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Pemerintah Tetapkan Tarif Listrik Oktober-Desember 2025, Ini DaftarnyaNews25 menit yang lalu</t>
+          <t>Dongkrak Talenta Catur, Telkomsel Umumkan Pemenang Chessnation 2025Lifestyle22 menit yang lalu</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -616,7 +624,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929075531-4-670921/pemerintah-tetapkan-tarif-listrik-oktober-desember-2025-ini-daftarnya</t>
+          <t>https://www.cnbcindonesia.com/lifestyle/20250929131324-33-671086/dongkrak-talenta-catur-telkomsel-umumkan-pemenang-chessnation-2025</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
@@ -624,7 +632,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Breaking! Rupiah Perkasa, Dolar AS Turun ke Rp16.640Market26 menit yang lalu</t>
+          <t>CNBC InsightMiliarder Pertama Dunia Kirim Uang Bantu RI Basmi Cacingan-Bangun WCEntrepreneur26 menit yang lalu</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -639,7 +647,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250929082543-17-670927/breaking-rupiah-perkasa-dolar-as-turun-ke-rp16640</t>
+          <t>https://www.cnbcindonesia.com/entrepreneur/20230929083409-25-476380/miliarder-pertama-dunia-kirim-uang-bantu-ri-basmi-cacingan-bangun-wc</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -647,7 +655,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>InternasionalRaja Singa Tiba-Tiba Meledak di Sini, Kasus Naik 460%News30 menit yang lalu</t>
+          <t>Contact Center Pegadaian Borong Penghargaan di Ajang ICCA 2025News28 menit yang lalu</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -662,7 +670,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929084616-4-670934/raja-singa-tiba-tiba-meledak-di-sini-kasus-naik-460</t>
+          <t>https://www.cnbcindonesia.com/news/20250929125412-4-671079/contact-center-pegadaian-borong-penghargaan-di-ajang-icca-2025</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -670,7 +678,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Netizen Teriak M-banking BCA &amp; blu Kompak Error, Ini Kata ManajemenMarket37 menit yang lalu</t>
+          <t>Kebakaran Data Center Hancur Dilahap Api, Layanan Publik Lumpuh TotalTech31 menit yang lalu</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -685,7 +693,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250929084732-17-670940/netizen-teriak-m-banking-bca-blu-kompak-error-ini-kata-manajemen</t>
+          <t>https://www.cnbcindonesia.com/tech/20250929121850-37-671058/kebakaran-data-center-hancur-dilahap-api-layanan-publik-lumpuh-total</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -693,7 +701,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Pertamina Bakal Gabung 3 Anak Usahanya, Ini Respons BahlilNews45 menit yang lalu</t>
+          <t>INET Umumkan Rights Issue, Incar Dana Segar Rp3,2 TriliunMarket36 menit yang lalu</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -708,7 +716,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929074918-4-670920/pertamina-bakal-gabung-3-anak-usahanya-ini-respons-bahlil</t>
+          <t>https://www.cnbcindonesia.com/market/20250929112514-17-671018/inet-umumkan-rights-issue-incar-dana-segar-rp32-triliun</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -716,7 +724,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Investor Tunggu Data Penting Australia, Bursa Asia Dibuka VariatifMarket52 menit yang lalu</t>
+          <t>Prabowo: Aku Tuh Terus Terang Aja Lho, Saya Nggak Dendam sama AniesNews38 menit yang lalu</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -731,15 +739,19 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250929082751-17-670929/investor-tunggu-data-penting-australia-bursa-asia-dibuka-variatif</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/news/20250929130421-4-671083/prabowo-aku-tuh-terus-terang-aja-lho-saya-nggak-dendam-sama-anies</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>prabowo</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Penyebab Keracunan MBG Dibeberkan Profesor Eks Direktur WHOTech55 menit yang lalu</t>
+          <t>Daebak! V BTS Dinobatkan Jadi Pria Paling Tampan di Dunia 2025Lifestyle41 menit yang lalu</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -754,19 +766,15 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250929083011-37-670928/penyebab-keracunan-mbg-dibeberkan-profesor-eks-direktur-who</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>mbg</t>
-        </is>
-      </c>
+          <t>https://www.cnbcindonesia.com/lifestyle/20250929120602-33-671059/daebak-v-bts-dinobatkan-jadi-pria-paling-tampan-di-dunia-2025</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Pelabuhan Tanjung Priok Bakal Dikepung Tol, Rute Terbaru Nempel JISNews1 jam yang lalu</t>
+          <t>Zulhas Cs Mau Kebut Kawasan Pangan Wanam, Ada Pengembangan Etanol-B50News42 menit yang lalu</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -781,7 +789,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250928193756-4-670880/pelabuhan-tanjung-priok-bakal-dikepung-tol-rute-terbaru-nempel-jis</t>
+          <t>https://www.cnbcindonesia.com/news/20250929123411-4-671063/zulhas-cs-mau-kebut-kawasan-pangan-wanam-ada-pengembangan-etanol-b50</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
@@ -789,7 +797,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Asing Terciduk Diam-diam Lego 10 Saham Ini Kala Cetak Net Buy JumboMarket1 jam yang lalu</t>
+          <t>Prabowo Klaim Usai Hapus 145 Aturan Soal Pupuk, ada yang PeringatkanNews44 menit yang lalu</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -804,15 +812,19 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250929081104-17-670923/asing-terciduk-diam-diam-lego-10-saham-ini-kala-cetak-net-buy-jumbo</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/news/20250929124914-4-671077/prabowo-klaim-usai-hapus-145-aturan-soal-pupuk-ada-yang-peringatkan</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>prabowo</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Triniti Land (TRIN) Jual Saham Anak Usaha, Ada Apa?Market1 jam yang lalu</t>
+          <t>Live Now! BPRS Buka-Bukaan Peluang dan Tantangan Ekonomi Syariah RINews46 menit yang lalu</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -827,7 +839,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250929082043-17-670926/triniti-land--trin--jual-saham-anak-usaha-ada-apa</t>
+          <t>https://www.cnbcindonesia.com/news/20250929120632-4-671040/live-now-bprs-buka-bukaan-peluang-dan-tantangan-ekonomi-syariah-ri</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
@@ -835,7 +847,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>BCA Mobile Down 2 Jam Ramai di Medsos, Netizen Curhat Susah ke KantorTech1 jam yang lalu</t>
+          <t>Baru Berlaku 2023, Kok UU P2SK Direvisi Lagi? Begini Penjelasannya!News50 menit yang lalu</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -850,7 +862,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250929080708-37-670924/bca-mobile-down-2-jam-ramai-di-medsos-netizen-curhat-susah-ke-kantor</t>
+          <t>https://www.cnbcindonesia.com/news/20250929102816-4-670987/baru-berlaku-2023-kok-uu-p2sk-direvisi-lagi-begini-penjelasannya</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -858,7 +870,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Catat! 5 Emiten Ini Tebar Dividen Pekan IniResearch1 jam yang lalu</t>
+          <t>Cerita Mamimu, Dari Dapur Rumah Hingga Perluas Pasar Berkat TASPENNews55 menit yang lalu</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -873,7 +885,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/research/20250929052328-128-670902/catat-5-emiten-ini-tebar-dividen-pekan-ini</t>
+          <t>https://www.cnbcindonesia.com/news/20250929124209-4-671070/cerita-mamimu-dari-dapur-rumah-hingga-perluas-pasar-berkat-taspen</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
@@ -881,7 +893,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Pertamina Siap Pasok Kebutuhan SPBU VIVO Hingga 40 Ribu Barel BBMNews1 jam yang lalu</t>
+          <t>Terungkap! Sepatu Impor KW Nike Cs di Senen-Jatinegara dari Negara IniNews56 menit yang lalu</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -896,7 +908,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929074116-4-670919/pertamina-siap-pasok-kebutuhan-spbu-vivo-hingga-40-ribu-barel-bbm</t>
+          <t>https://www.cnbcindonesia.com/news/20250929111144-4-671008/terungkap-sepatu-impor-kw-nike-cs-di-senen-jatinegara-dari-negara-ini</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
@@ -904,7 +916,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>InternasionalChina-Korut "Bersatu", Xi Jinping-Kim Jong Un Beri Pesan Baru ke DuniaNews1 jam yang lalu</t>
+          <t>Cara Cek Bansos Rp 600 Ribu Pakai KTP, Oktober Mulai CairTech59 menit yang lalu</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -919,7 +931,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929070953-4-670907/china-korut-bersatu-xi-jinping-kim-jong-un-beri-pesan-baru-ke-dunia</t>
+          <t>https://www.cnbcindonesia.com/tech/20250929123352-37-671069/cara-cek-bansos-rp-600-ribu-pakai-ktp-oktober-mulai-cair</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
@@ -927,7 +939,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>4 Poin Penting Dibahas Purbaya &amp; Bos BI Saat Santap Bebek GorengMarket1 jam yang lalu</t>
+          <t>Diburu Interpol, Ini Profil Duo Buron Kasus Keuangan RI Paling DicariMarket1 jam yang lalu</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -942,19 +954,15 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250929071811-17-670910/4-poin-penting-dibahas-purbaya-bos-bi-saat-santap-bebek-goreng</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>purbaya</t>
-        </is>
-      </c>
+          <t>https://www.cnbcindonesia.com/market/20250929110315-17-671004/diburu-interpol-ini-profil-duo-buron-kasus-keuangan-ri-paling-dicari</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Revisi UU BUMN Akan Disahkan DPR Pekan Ini, Ini 11 Poin PentingMarket1 jam yang lalu</t>
+          <t>Prabowo Umumkan Akan Segera Bangun Tanggul Laut Raksasa di PanturaNews1 jam yang lalu</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -969,15 +977,19 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250929074512-17-670922/revisi-uu-bumn-akan-disahkan-dpr-pekan-ini-ini-11-poin-penting</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/news/20250929123959-4-671067/prabowo-umumkan-akan-segera-bangun-tanggul-laut-raksasa-di-pantura</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>prabowo</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Purbaya Bicara Soal Nasib BI di RUU P2SK, Hilang Independensi?Market1 jam yang lalu</t>
+          <t>5 Bahaya HP Jarang Update iOS di iPhone dan OS di AndroidTech1 jam yang lalu</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -992,19 +1004,15 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250928234637-17-670898/purbaya-bicara-soal-nasib-bi-di-ruu-p2sk-hilang-independensi</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>purbaya</t>
-        </is>
-      </c>
+          <t>https://www.cnbcindonesia.com/tech/20250929111544-37-671012/5-bahaya-hp-jarang-update-ios-di-iphone-dan-os-di-android</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Asing Net Buy 7,38 T Pekan Lalu, Kompak Borong 10 Saham IniMarket1 jam yang lalu</t>
+          <t>Saham PGUN Haji Isam OTW Jadi Raja Konsumer RI, HMSP-UNVR-AMRT LewatMarket1 jam yang lalu</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1019,7 +1027,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250929073515-17-670918/asing-net-buy-738-t-pekan-lalu-kompak-borong-10-saham-ini</t>
+          <t>https://www.cnbcindonesia.com/market/20250929105938-17-671000/saham-pgun-haji-isam-otw-jadi-raja-konsumer-ri-hmsp-unvr-amrt-lewat</t>
         </is>
       </c>
       <c r="E25" t="inlineStr"/>
@@ -1027,7 +1035,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Langit Tiba-Tiba Terang Benderang Bikin Panik, Ternyata Kelakuan ChinaTech1 jam yang lalu</t>
+          <t>Ekspor RI ke UE-Kanada Bakal Melejit 2 Kali Lipat, Ini PemicunyaNews1 jam yang lalu</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1042,7 +1050,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250928224447-37-670894/langit-tiba-tiba-terang-benderang-bikin-panik-ternyata-kelakuan-china</t>
+          <t>https://www.cnbcindonesia.com/news/20250929115812-4-671039/ekspor-ri-ke-ue-kanada-bakal-melejit-2-kali-lipat-ini-pemicunya</t>
         </is>
       </c>
       <c r="E26" t="inlineStr"/>
@@ -1050,7 +1058,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>InternasionalKala Bumi Ngamuk ke Netanyahu: Demo Massal-Lempar SepatuNews1 jam yang lalu</t>
+          <t>Studi Ungkap 13 Ciri Psikopat yang Bisa Dikenali sebelum DewasaLifestyle1 jam yang lalu</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1065,7 +1073,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929073240-4-670917/kala-bumi-ngamuk-ke-netanyahu-demo-massal-lempar-sepatu</t>
+          <t>https://www.cnbcindonesia.com/lifestyle/20250929111337-33-671010/studi-ungkap-13-ciri-psikopat-yang-bisa-dikenali-sebelum-dewasa</t>
         </is>
       </c>
       <c r="E27" t="inlineStr"/>
@@ -1073,7 +1081,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Fenomena Langka: China &amp; Singapura Berlomba-Lomba Akuisisi Emiten RIResearch2 jam yang lalu</t>
+          <t>IHSG Sesi I Naik 0,6%,Market Cap Tembus Rp 15.000 TriliunMarket1 jam yang lalu</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1088,7 +1096,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/research/20250926132341-128-670474/fenomena-langka-china-singapura-berlomba-lomba-akuisisi-emiten-ri</t>
+          <t>https://www.cnbcindonesia.com/market/20250929114719-17-671029/ihsg-sesi-i-naik-06market-cap-tembus-rp-15000-triliun</t>
         </is>
       </c>
       <c r="E28" t="inlineStr"/>
@@ -1096,7 +1104,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Modus Baru Penipuan Incar Karyawan Pakai OTP, Google Ungkap Cara CegahTech2 jam yang lalu</t>
+          <t>Avanza-Veloz Hybrid Bakal Hadir di RI? Ini Bocoran dari ToyotaNews1 jam yang lalu</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1111,7 +1119,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250928225023-37-670895/modus-baru-penipuan-incar-karyawan-pakai-otp-google-ungkap-cara-cegah</t>
+          <t>https://www.cnbcindonesia.com/news/20250929111022-4-671007/avanza-veloz-hybrid-bakal-hadir-di-ri-ini-bocoran-dari-toyota</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
@@ -1119,7 +1127,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>InternasionalAS di Ujung Tanduk, Trump Warning PHK PNS Besar-besaranNews2 jam yang lalu</t>
+          <t>2 dari 3 Petani RI Berusia Tua, Siapa yang Menanam Padi?Research1 jam yang lalu</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1134,7 +1142,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929063500-4-670906/as-di-ujung-tanduk-trump-warning-phk-pns-besar-besaran</t>
+          <t>https://www.cnbcindonesia.com/research/20250926150159-128-670516/2-dari-3-petani-ri-berusia-tua-siapa-yang-menanam-padi</t>
         </is>
       </c>
       <c r="E30" t="inlineStr"/>
@@ -1142,7 +1150,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Anggito Jadi Ketua LPS, Purbaya Usul ke Prabowo Tak Tambah Wamen LagiMarket2 jam yang lalu</t>
+          <t>Purbaya Terima Kritik Rocky Gerung, Tapi Harus Minta Maaf Kalau SalahNews1 jam yang lalu</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1157,7 +1165,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250928230107-17-670896/anggito-jadi-ketua-lps-purbaya-usul-ke-prabowo-tak-tambah-wamen-lagi</t>
+          <t>https://www.cnbcindonesia.com/news/20250929114309-4-671027/purbaya-terima-kritik-rocky-gerung-tapi-harus-minta-maaf-kalau-salah</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1169,7 +1177,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>RI Nomor Satu Paling Parah Sedunia, Harus Belajar dari JepangTech2 jam yang lalu</t>
+          <t>Raksasa Tekstil di Bandung Pailit, Sudah Setop Operasi Sejak 2024Market1 jam yang lalu</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1184,7 +1192,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250928223656-37-670893/ri-nomor-satu-paling-parah-sedunia-harus-belajar-dari-jepang</t>
+          <t>https://www.cnbcindonesia.com/market/20250929120928-17-671044/raksasa-tekstil-di-bandung-pailit-sudah-setop-operasi-sejak-2024</t>
         </is>
       </c>
       <c r="E32" t="inlineStr"/>
@@ -1192,7 +1200,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>InternasionalPrabowo Bertemu 'Empat Mata' Dengan Trump di Sidang PBB, Katakan IniNews2 jam yang lalu</t>
+          <t>Prabowo Ungkap ada 'Harta Karun' Dibalik Limbah TimahNews1 jam yang lalu</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1207,15 +1215,19 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929054354-4-670905/prabowo-bertemu-empat-mata-dengan-trump-di-sidang-pbb-katakan-ini</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/news/20250929114953-4-671031/prabowo-ungkap-ada-harta-karun-dibalik-limbah-timah</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>prabowo</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Harga Emas Bisa Tembus Langit Pekan Ini Tapi Ada 3 SyaratnyaResearch2 jam yang lalu</t>
+          <t>Lebih dari 100 Lapangan Padel Bangkrut, Dulu Viral sekarang SuramLifestyle1 jam yang lalu</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1230,7 +1242,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/research/20250929051305-128-670901/harga-emas-bisa-tembus-langit-pekan-ini-tapi-ada-3-syaratnya</t>
+          <t>https://www.cnbcindonesia.com/lifestyle/20250929105342-33-670996/lebih-dari-100-lapangan-padel-bangkrut-dulu-viral-sekarang-suram</t>
         </is>
       </c>
       <c r="E34" t="inlineStr"/>
@@ -1238,7 +1250,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Fitur Chat WhatsApp Tanpa Nomor Telepon, Cara dan LarangannyaTech3 jam yang lalu</t>
+          <t>InternasionalPetaka Hantam Tetangga RI, Bandara Ditutup-Ribuan Orang DievakuasiNews1 jam yang lalu</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1253,7 +1265,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250928222748-37-670891/fitur-chat-whatsapp-tanpa-nomor-telepon-cara-dan-larangannya</t>
+          <t>https://www.cnbcindonesia.com/news/20250929113831-4-671021/petaka-hantam-tetangga-ri-bandara-ditutup-ribuan-orang-dievakuasi</t>
         </is>
       </c>
       <c r="E35" t="inlineStr"/>
@@ -1261,7 +1273,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Purbaya: Saya Koboi, Pistolnya Banyak Tapi Gak SembaranganMarket3 jam yang lalu</t>
+          <t>Prabowo ke PKS: 2 Kali Dukung 2 Kali Kalah, Giliran Menang Gak DukungNews1 jam yang lalu</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1276,19 +1288,19 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250928223403-17-670892/purbaya-saya-koboi-pistolnya-banyak-tapi-gak-sembarangan</t>
+          <t>https://www.cnbcindonesia.com/news/20250929115030-4-671041/prabowo-ke-pks-2-kali-dukung-2-kali-kalah-giliran-menang-gak-dukung</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>purbaya</t>
+          <t>prabowo</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>InternasionalSanksi Barat Gak Mempan, Putin Garap Proyek Nuklir Rp 400 T di IranNews3 jam yang lalu</t>
+          <t>Telkom, Telkomsel, Indosat, XLSmart Pilih Dian Siswarini Ketua ATSITech1 jam yang lalu</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1303,7 +1315,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929053949-4-670904/sanksi-barat-gak-mempan-putin-garap-proyek-nuklir-rp-400-t-di-iran</t>
+          <t>https://www.cnbcindonesia.com/tech/20250929113231-37-671024/telkom-telkomsel-indosat-xlsmart-pilih-dian-siswarini-ketua-atsi</t>
         </is>
       </c>
       <c r="E37" t="inlineStr"/>
@@ -1311,7 +1323,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>NewsletterWaspada! 7 Isu Penting Bisa Bikin IHSG &amp; Rupiah 'Keringetan' Pekan IniResearch3 jam yang lalu</t>
+          <t>MMIX Bakal Bagikan Saham Bonus 1:1 Cek Jadwalnya!Market1 jam yang lalu</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1326,7 +1338,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/research/20250929050437-128-670900/waspada-7-isu-penting-bisa-bikin-ihsg-rupiah-keringetan-pekan-ini</t>
+          <t>https://www.cnbcindonesia.com/market/20250929115719-17-671038/mmix-bakal-bagikan-saham-bonus-11-cek-jadwalnya</t>
         </is>
       </c>
       <c r="E38" t="inlineStr"/>
@@ -1334,7 +1346,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>InternasionalHoror Penembakan Sadis di Ibadah Minggu Gereja AS, Ada Korban TewasNews4 jam yang lalu</t>
+          <t>Sepatu Impor Nike Cs di Senen-Jatinegara Barang KW-Harga di Luar NalarNews1 jam yang lalu</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1349,7 +1361,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929043856-4-670899/horor-penembakan-sadis-di-ibadah-minggu-gereja-as-ada-korban-tewas</t>
+          <t>https://www.cnbcindonesia.com/news/20250929105022-4-670995/sepatu-impor-nike-cs-di-senen-jatinegara-barang-kw-harga-di-luar-nalar</t>
         </is>
       </c>
       <c r="E39" t="inlineStr"/>
@@ -1357,7 +1369,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Prabowo Rapat Bareng Menteri Minggu Sore, Bahas MBG hingga Stok BerasNews9 jam yang lalu</t>
+          <t>InternasionalPutin Menggila! Rusia Tembak 595 Drone 'Bakar' Kyiv, Jet NATO TurunNews1 jam yang lalu</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1372,19 +1384,15 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250928233141-4-670897/prabowo-rapat-bareng-menteri-minggu-sore-bahas-mbg-hingga-stok-beras</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>mbg</t>
-        </is>
-      </c>
+          <t>https://www.cnbcindonesia.com/news/20250929111809-4-671013/putin-menggila-rusia-tembak-595-drone-bakar-kyiv-jet-nato-turun</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>InternasionalDemonstrasi Berujung Maut, 39 Orang Tewas karena Berdesakan-TerinjakNews11 jam yang lalu</t>
+          <t>Prabowo Ungkit Rusuh 29 Agustus: Ada Keterlibatan Kekuatan TertentuNews1 jam yang lalu</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1399,15 +1407,19 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250928190245-4-670876/demonstrasi-berujung-maut-39-orang-tewas-karena-berdesakan-terinjak</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/news/20250929114729-4-671030/prabowo-ungkit-rusuh-29-agustus-ada-keterlibatan-kekuatan-tertentu</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>prabowo</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Haji Isam Punya Harta Rp 101 Triliun tapi Tak Masuk Forbes, Kok Bisa?Market11 jam yang lalu</t>
+          <t>DAIKIN Resmikan Pusat Keunggulan Pertama di BekasiNews1 jam yang lalu</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1422,7 +1434,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250928193130-17-670879/haji-isam-punya-harta-rp-101-triliun-tapi-tak-masuk-forbes-kok-bisa</t>
+          <t>https://www.cnbcindonesia.com/news/20250929114311-4-671028/daikin-resmikan-pusat-keunggulan-pertama-di-bekasi</t>
         </is>
       </c>
       <c r="E42" t="inlineStr"/>
@@ -1430,7 +1442,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>InternasionalMedia Malaysia Soroti Transportasi Jakarta Ungguli Kuala LumpurNews12 jam yang lalu</t>
+          <t>Penutupan Munas VI PKSPrabowo Lapor Penerima MBG Dekati 30 Juta, Akui ada Keracunan MakananNews1 jam yang lalu</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1445,15 +1457,19 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250928192227-4-670878/media-malaysia-soroti-transportasi-jakarta-ungguli-kuala-lumpur</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/news/20250929100637-4-670965/prabowo-lapor-penerima-mbg-dekati-30-juta-akui-ada-keracunan-makanan</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>mbg</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Marak Penipuan Pakai Modus Baru Catphishing, Ini Tips HindariTech12 jam yang lalu</t>
+          <t>Harga Minyak Tergelincir Awal Pekan, Brent Kembali ke Bawah US$70Market1 jam yang lalu</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1468,7 +1484,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250928191555-37-670877/marak-penipuan-pakai-modus-baru-catphishing-ini-tips-hindari</t>
+          <t>https://www.cnbcindonesia.com/market/20250929102957-17-670983/harga-minyak-tergelincir-awal-pekan-brent-kembali-ke-bawah-us-70</t>
         </is>
       </c>
       <c r="E44" t="inlineStr"/>
@@ -1476,7 +1492,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Menkes Ajak Sarapan 2 Telur Rebus Bukan Nasi Uduk-Bubur, Ini AlasannyaLifestyle12 jam yang lalu</t>
+          <t>Rupiah Anjlok 20% vs Real Arab, Umroh Bawa Rp 10 Juta Langsung MiskinResearch2 jam yang lalu</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1491,7 +1507,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/lifestyle/20250928184201-33-670873/menkes-ajak-sarapan-2-telur-rebus-bukan-nasi-uduk-bubur-ini-alasannya</t>
+          <t>https://www.cnbcindonesia.com/research/20250929102709-128-670989/rupiah-anjlok-20-vs-real-arab-umroh-bawa-rp-10-juta-langsung-miskin</t>
         </is>
       </c>
       <c r="E45" t="inlineStr"/>
@@ -1499,7 +1515,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>14.341 Tiket KA Rp 80.000 Gagal Dijual, Tenang! Masih Ada Diskon 20%News12 jam yang lalu</t>
+          <t>Prabowo Titahkan TNI-Polri Operasi Besar-Besaran di Babel, Ada Apa?News2 jam yang lalu</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1514,15 +1530,19 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250928181323-4-670859/14341-tiket-ka-rp-80000-gagal-dijual-tenang-masih-ada-diskon-20</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/news/20250929113914-4-671023/prabowo-titahkan-tni-polri-operasi-besar-besaran-di-babel-ada-apa</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>prabowo</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Nabi Musa Bisa Membelah Laut Merah, Begini Penjelasan IlmiahnyaTech13 jam yang lalu</t>
+          <t>Pengumuman! Bakal Ada Sistem Baru, Ekspor Bakal Makin MudahNews2 jam yang lalu</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1537,7 +1557,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250928175524-37-670858/nabi-musa-bisa-membelah-laut-merah-begini-penjelasan-ilmiahnya</t>
+          <t>https://www.cnbcindonesia.com/news/20250929112225-4-671014/pengumuman-bakal-ada-sistem-baru-ekspor-bakal-makin-mudah</t>
         </is>
       </c>
       <c r="E47" t="inlineStr"/>
@@ -1545,7 +1565,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Lewat Inovasi, Anak Usaha InJourney Raih Penghargaan di Ajang Ini!News13 jam yang lalu</t>
+          <t>Jelang Merger dengan ADMF, Bursa Gembok Saham MFINMarket2 jam yang lalu</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1560,7 +1580,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250928201250-4-670882/lewat-inovasi-anak-usaha-injourney-raih-penghargaan-di-ajang-ini</t>
+          <t>https://www.cnbcindonesia.com/market/20250929083437-17-670930/jelang-merger-dengan-admf-bursa-gembok-saham-mfin</t>
         </is>
       </c>
       <c r="E48" t="inlineStr"/>
@@ -1568,7 +1588,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Makanan Murah Ini Bagus Buat Ibu Hamil dan Cegah Bayi StuntingLifestyle13 jam yang lalu</t>
+          <t>Dibongkar Prabowo! 80% Produksi Timah RI Ternyata DiselundupkanNews2 jam yang lalu</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1583,15 +1603,19 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/lifestyle/20250928171845-33-670849/makanan-murah-ini-bagus-buat-ibu-hamil-dan-cegah-bayi-stunting</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/news/20250929113128-4-671020/dibongkar-prabowo-80-produksi-timah-ri-ternyata-diselundupkan</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>prabowo</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Rahasia Satelit Bertahan Mengorbit di Angkasa Terungkap, Ternyata IniTech13 jam yang lalu</t>
+          <t>Penutupan Munas VI PKSPrabowo Geram Korupsi di RI Parah: Orang Pintar itu Sering Nyolong!News2 jam yang lalu</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1606,7 +1630,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250928165143-37-670848/rahasia-satelit-bertahan-mengorbit-di-angkasa-terungkap-ternyata-ini</t>
+          <t>https://www.cnbcindonesia.com/news/20250929100720-4-670966/prabowo-geram-korupsi-di-ri-parah-orang-pintar-itu-sering-nyolong</t>
         </is>
       </c>
       <c r="E50" t="inlineStr"/>
@@ -1614,7 +1638,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Siap-Siap! Rumah Murah Bakal Dibangun di Jakarta, Ini BocorannyaNews13 jam yang lalu</t>
+          <t>Waspada Angin Kencang Hantam Jakarta, Cek Peringatan Baru BMKGTech2 jam yang lalu</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1629,7 +1653,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250928133943-4-670813/siap-siap-rumah-murah-bakal-dibangun-di-jakarta-ini-bocorannya</t>
+          <t>https://www.cnbcindonesia.com/tech/20250929105759-37-670998/waspada-angin-kencang-hantam-jakarta-cek-peringatan-baru-bmkg</t>
         </is>
       </c>
       <c r="E51" t="inlineStr"/>
@@ -1637,7 +1661,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Tol RI Tambah Panjang Lagi 308,7 Km Tahun Depan, Tembus Yogya &amp; KediriNews14 jam yang lalu</t>
+          <t>Prabowo: Sebagian Besar Rakyat Kita Belum Menikmati Kekayaan IndonesiaNews2 jam yang lalu</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1652,15 +1676,19 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250927210807-4-670751/tol-ri-tambah-panjang-lagi-3087-km-tahun-depan-tembus-yogya-kediri</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/news/20250929112012-4-671017/prabowo-sebagian-besar-rakyat-kita-belum-menikmati-kekayaan-indonesia</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>prabowo</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Ada 9 Fenomena Langit di Oktober, Muncul Hujan Meteor-SupermoonResearch14 jam yang lalu</t>
+          <t>Prabowo Sebut Ada 1.000 Tambang Timah Ilegal di Bangka BelitungNews2 jam yang lalu</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1675,15 +1703,19 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/research/20250928151602-128-670840/ada-9-fenomena-langit-di-oktober-muncul-hujan-meteor-supermoon</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/news/20250929102429-4-671015/prabowo-sebut-ada-1000-tambang-timah-ilegal-di-bangka-belitung</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>prabowo</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Peran &amp; Tantangan BPRS dalam Mendorong Ekonomi Syariah di IndonesiaNews14 jam yang lalu</t>
+          <t>14 Makanan Sehari-Hari yang Mengandung Mikroplastik, Ada Favorit Kamu?Lifestyle2 jam yang lalu</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1698,7 +1730,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250928185539-4-670875/peran-tantangan-bprs-dalam-mendorong-ekonomi-syariah-di-indonesia</t>
+          <t>https://www.cnbcindonesia.com/lifestyle/20250929103251-33-670986/14-makanan-sehari-hari-yang-mengandung-mikroplastik-ada-favorit-kamu</t>
         </is>
       </c>
       <c r="E54" t="inlineStr"/>
@@ -1706,7 +1738,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Jalur Kereta Api Mati Mau Dihidupkan Lagi, Ini DaftarnyaNews14 jam yang lalu</t>
+          <t>Wah! Purbaya Tiba-tiba Sidak Kantor BNINews2 jam yang lalu</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1721,15 +1753,19 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250927214927-4-670762/jalur-kereta-api-mati-mau-dihidupkan-lagi-ini-daftarnya</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/news/20250929110139-4-671001/wah-purbaya-tiba-tiba-sidak-kantor-bni</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>purbaya</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Sentimen Pekan DepanWaspada! IHSG &amp; Rupiah Rawan Bergejolak karena Kabar dari AS dan ChinaResearch14 jam yang lalu</t>
+          <t>Mundur dari Direktur Bank Permata, Abdy Dharma Pindah ke Bangkok BankMarket2 jam yang lalu</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1744,7 +1780,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/research/20250928033702-128-670771/waspada-ihsg-rupiah-rawan-bergejolak-karena-kabar-dari-as-dan-china</t>
+          <t>https://www.cnbcindonesia.com/market/20250929091636-17-670956/mundur-dari-direktur-bank-permata-abdy-dharma-pindah-ke-bangkok-bank</t>
         </is>
       </c>
       <c r="E56" t="inlineStr"/>
@@ -1752,7 +1788,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Ada Tol Baru, Warga BSD ke Bogor Terasa SejengkalNews15 jam yang lalu</t>
+          <t>InternasionalTerima Duit Suap Rp 626 M, Eks Mentan Dihukum Mati di SiniNews2 jam yang lalu</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1767,7 +1803,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250927211218-4-670753/ada-tol-baru-warga-bsd-ke-bogor-terasa-sejengkal</t>
+          <t>https://www.cnbcindonesia.com/news/20250929103511-4-670988/terima-duit-suap-rp-626-m-eks-mentan-dihukum-mati-di-sini</t>
         </is>
       </c>
       <c r="E57" t="inlineStr"/>
@@ -1775,7 +1811,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Megathrust Meledak, Yogya Bisa Diguncang Gempa M 8,8-Digulung TsunamiTech15 jam yang lalu</t>
+          <t>Penutupan Munas VI PKSKelakar Prabowo: PKS Gabung Usai Merantau, Usul Prof ITB Jadi MenteriNews2 jam yang lalu</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1790,15 +1826,19 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250928150121-37-670839/megathrust-meledak-yogya-bisa-diguncang-gempa-m-88-digulung-tsunami</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/news/20250929110348-4-671003/kelakar-prabowo-pks-gabung-usai-merantau-usul-prof-itb-jadi-menteri</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>prabowo</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>CNBC InsightPresiden RI Tolak Sosok Ini Jadi Menteri karena Idenya Terlalu GilaEntrepreneur15 jam yang lalu</t>
+          <t>BI Luncurkan Matchmaking Overnight Index Swap, Ini TujuannyaNews2 jam yang lalu</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1813,7 +1853,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/entrepreneur/20250927214356-25-670761/presiden-ri-tolak-sosok-ini-jadi-menteri-karena-idenya-terlalu-gila</t>
+          <t>https://www.cnbcindonesia.com/news/20250929105725-4-670997/bi-luncurkan-matchmaking-overnight-index-swap-ini-tujuannya</t>
         </is>
       </c>
       <c r="E59" t="inlineStr"/>
@@ -1821,7 +1861,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Proyek Tol Puncak Dilelang Tahun Depan, Begini Rencana RutenyaNews15 jam yang lalu</t>
+          <t>Dunia Makin Menyeramkan, Prabowo Ungkap Ketakutan Besar Eropa!News2 jam yang lalu</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1836,15 +1876,19 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250927212212-4-670755/proyek-tol-puncak-dilelang-tahun-depan-begini-rencana-rutenya</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/news/20250929110147-4-671002/dunia-makin-menyeramkan-prabowo-ungkap-ketakutan-besar-eropa</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>prabowo</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Mobil Ini Paling Gak Laku di RI, Cuma Terjual 1 UnitNews16 jam yang lalu</t>
+          <t>Memahami Ragam Sistem Pendidikan Global, Studi Kasus Gibran RakabumingOpini2 jam yang lalu</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1859,10 +1903,708 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250927215850-4-670765/mobil-ini-paling-gak-laku-di-ri-cuma-terjual-1-unit</t>
+          <t>https://www.cnbcindonesia.com/opini/20250929094358-14-670959/memahami-ragam-sistem-pendidikan-global-studi-kasus-gibran-rakabuming</t>
         </is>
       </c>
       <c r="E61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>InternasionalMedia Asing Tiba-Tiba Sorot Bali, Sebut Jadi KorbanNews2 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/news/20250929102035-4-670968/media-asing-tiba-tiba-sorot-bali-sebut-jadi-korban</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Wismilak Inti Makmur (WIIM) Bakal Lepas 24 Juta Saham TreasuriMarket2 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/market/20250929093056-17-670957/wismilak-inti-makmur--wiim--bakal-lepas-24-juta-saham-treasuri</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Penutupan Munas VI PKSPrabowo Tutup Munas VI PKS: Angka 8 itu Selalu Hadir di Hidup SayaNews2 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/news/20250929100526-4-670964/prabowo-tutup-munas-vi-pks-angka-8-itu-selalu-hadir-di-hidup-saya</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Robot Tesla Pembawa Maut, Manusia Hampir MeninggalTech2 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/tech/20250929101735-37-670967/robot-tesla-pembawa-maut-manusia-hampir-meninggal</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Terungkap Jenis Bakteri 'Biang Kerok' Keracunan MBG di Bandung BaratLifestyle3 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/lifestyle/20250929095828-33-670962/terungkap-jenis-bakteri-biang-kerok-keracunan-mbg-di-bandung-barat</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>mbg</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>RI Punya Harta Karun Bernilai Fantastis, Tapi Malah Dibuang!News3 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/news/20250929095936-4-670963/ri-punya-harta-karun-bernilai-fantastis-tapi-malah-dibuang</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>6 Gerbang Tol Dalam Kota Ditutup Mulai Hari iniNews3 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/news/20250929102057-4-670984/6-gerbang-tol-dalam-kota-ditutup-mulai-hari-ini</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Bos EXCL Borong Saham Perusahaan Rp 1,59 MiliarMarket3 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/market/20250929091656-17-670952/bos-excl-borong-saham-perusahaan-rp-159-miliar</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr"/>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>United Tractors (UNTR) Bagi Dividen Interim Rp2,05 T, Ini JadwalnyaMarket3 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/market/20250929101457-17-670969/united-tractors--untr--bagi-dividen-interim-rp205-t-ini-jadwalnya</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr"/>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Bursa Gembok Perdagangan Saham 7 Emiten IniMarket3 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/market/20250929095117-17-670960/bursa-gembok-perdagangan-saham-7-emiten-ini</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr"/>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Deretan Emiten "Harta Karun", Anda Bisa Jadi Crazy Rich dalam 10 TahunResearch3 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/research/20250926130822-128-670465/deretan-emiten-harta-karun-anda-bisa-jadi-crazy-rich-dalam-10-tahun</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr"/>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Alasan Ilmiah Daging Hiu Tak Boleh Dimakan, Bukan Cuma Tinggi MerkuriTech3 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/tech/20250929095807-37-670961/alasan-ilmiah-daging-hiu-tak-boleh-dimakan-bukan-cuma-tinggi-merkuri</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr"/>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Prabowo Mau Pindahkan 9.500 ASN ke IKN hingga 2029, Begini TahapannyaNews3 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/news/20250929084917-4-670939/prabowo-mau-pindahkan-9500-asn-ke-ikn-hingga-2029-begini-tahapannya</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>prabowo</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>12 Buah dan Sayuran 'Kotor' yang Mengandung Pestisida Paling TinggiLifestyle3 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/lifestyle/20250929090606-33-670949/12-buah-dan-sayuran-kotor-yang-mengandung-pestisida-paling-tinggi</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Waskita Karya Infrastruktur Umumkan Jual Anak Usaha Rp179,99 MiliarMarket3 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/market/20250929084954-17-670947/waskita-karya-infrastruktur-umumkan-jual-anak-usaha-rp17999-miliar</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr"/>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Interpol Buru Bos WanaArtha &amp; Kresna Group usai Ciduk Adrian GunadiMarket3 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/market/20250929092533-17-670955/interpol-buru-bos-wanaartha-kresna-group-usai-ciduk-adrian-gunadi</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr"/>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>7 Aplikasi Kamera HP Buat Hasilkan Foto Setara DSLR, Cek DaftarnyaTech4 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/tech/20250929092522-37-670954/7-aplikasi-kamera-hp-buat-hasilkan-foto-setara-dslr-cek-daftarnya</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr"/>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Besok, Malaysia Resmi Turunkan Harga BBM RON 95 Jadi Rp7.849 per LiterNews4 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/news/20250929094011-4-670958/besok-malaysia-resmi-turunkan-harga-bbm-ron-95-jadi-rp7849-per-liter</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr"/>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Asia Pukul Balik Amerika: Dolar AS Ditendang, Won - Rupiah Jadi RajaResearch4 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/research/20250929091330-128-670951/asia-pukul-balik-amerika-dolar-as-ditendang-won--rupiah-jadi-raja</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr"/>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>5 Waktu Terbaik Makan Pisang yang Tak Banyak Orang TahuLifestyle4 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/lifestyle/20250928140454-33-670827/5-waktu-terbaik-makan-pisang-yang-tak-banyak-orang-tahu</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr"/>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Harga Saham Bergerak Tak Wajar, BEI Pantau Ketat 5 Emiten IniMarket4 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/market/20250929090519-17-670948/harga-saham-bergerak-tak-wajar-bei-pantau-ketat-5-emiten-ini</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr"/>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Asing Bawa Kabur Rp 42 T, Risiko Gagal Bayar RI Naik DrastisResearch4 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/research/20250929081207-128-670925/asing-bawa-kabur-rp-42-t-risiko-gagal-bayar-ri-naik-drastis</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr"/>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Daftar Bunga Deposito Rupiah &amp; Dolar BRI, BNI-Mandiri per 29 SeptemberResearch4 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/research/20250929053349-128-670903/daftar-bunga-deposito-rupiah-dolar-bri-bni-mandiri-per-29-september</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr"/>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Sepatu Impor Serang Pasar Senen dan Jatinegara, Mereknya Bikin KagetNews4 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/news/20250928200659-4-670881/sepatu-impor-serang-pasar-senen-dan-jatinegara-mereknya-bikin-kaget</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr"/>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Rekor Lagi! Harga Emas Antam Logam Mulia Hari Ini Hampir Rp 2,2 JutaResearch4 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/research/20250929083802-128-670932/rekor-lagi-harga-emas-antam-logam-mulia-hari-ini-hampir-rp-22-juta</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr"/>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Bank Syariah Nasional Resmi Dapat Izin Operasi dari OJKMarket4 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/market/20250929090720-17-670950/bank-syariah-nasional-resmi-dapat-izin-operasi-dari-ojk</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr"/>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>IHSG Dibuka Menguat, Balik Lagi ke Level 8.100Market4 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/market/20250929084220-17-670933/ihsg-dibuka-menguat-balik-lagi-ke-level-8100</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr"/>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Pemerintah Tetapkan Tarif Listrik Oktober-Desember 2025, Ini DaftarnyaNews4 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/news/20250929075531-4-670921/pemerintah-tetapkan-tarif-listrik-oktober-desember-2025-ini-daftarnya</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr"/>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Breaking! Rupiah Perkasa, Dolar AS Turun ke Rp16.640Market4 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/market/20250929082543-17-670927/breaking-rupiah-perkasa-dolar-as-turun-ke-rp16640</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr"/>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>InternasionalRaja Singa Tiba-Tiba Meledak di Sini, Kasus Naik 460%News4 jam yang lalu</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>https://www.cnbcindonesia.com/news/20250929084616-4-670934/raja-singa-tiba-tiba-meledak-di-sini-kasus-naik-460</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
SEL 3 - OK, kurang judulnya.
</commit_message>
<xml_diff>
--- a/daftar_berita/cnbc.xlsx
+++ b/daftar_berita/cnbc.xlsx
@@ -463,12 +463,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Prabowo Selamatkan Rp22 Triliun Duit Negara dari Tambang Timah IlegalNews1 menit yang lalu</t>
+          <t>InternasionalTrump Makin Gencar "Invasi" Negeri Sendiri, Kota Ini Siap MelawanNews4 menit yang lalu</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -478,24 +478,20 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929121348-4-671056/prabowo-selamatkan-rp22-triliun-duit-negara-dari-tambang-timah-ilegal</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>prabowo</t>
-        </is>
-      </c>
+          <t>https://www.cnbcindonesia.com/news/20250930122006-4-671480/trump-makin-gencar-invasi-negeri-sendiri-kota-ini-siap-melawan</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Ini 10 Bank Syariah Penyokong Ekonomi RakyatNews4 menit yang lalu</t>
+          <t>Wamenperin Sebut Produsen Rokok Tak Nikmati Kenaikan Harga, kok bisa?News9 menit yang lalu</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -505,7 +501,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929133640-4-671110/ini-10-bank-syariah-penyokong-ekonomi-rakyat</t>
+          <t>https://www.cnbcindonesia.com/news/20250930121920-4-671479/wamenperin-sebut-produsen-rokok-tak-nikmati-kenaikan-harga-kok-bisa</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -513,12 +509,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Surge (WIFI) Kompak Divestasi Saham 3 Anak UsahaMarket6 menit yang lalu</t>
+          <t>Survei Terbaru: Ojol Lebih Suka Potongan 20% untuk Promo &amp; InsentifTech13 menit yang lalu</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -528,7 +524,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250929083947-17-670931/surge--wifi--kompak-divestasi-saham-3-anak-usaha</t>
+          <t>https://www.cnbcindonesia.com/tech/20250930132454-37-671531/survei-terbaru-ojol-lebih-suka-potongan-20-untuk-promo-insentif</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -536,12 +532,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Pelajaran Pahit China &amp; India: MBG di RI Bisa Meledak Jadi Tragedi?Research11 menit yang lalu</t>
+          <t>Purbaya Tegur BUMN: Hati-Hati Salurkan Subsidi!News14 menit yang lalu</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -551,24 +547,24 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/research/20250929105903-128-670999/pelajaran-pahit-china-india-mbg-di-ri-bisa-meledak-jadi-tragedi</t>
+          <t>https://www.cnbcindonesia.com/news/20250930114905-4-671464/purbaya-tegur-bumn-hati-hati-salurkan-subsidi</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>mbg</t>
+          <t>purbaya</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Pegadaian dan Masjid Salman ITB Daur Ulang Air Hujan dan Air WudhuNews14 menit yang lalu</t>
+          <t>Sulap Sampah Jadi Energi, Bos Danantara Beberkan ManfaatnyaMarket18 menit yang lalu</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -578,7 +574,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929132227-4-671094/pegadaian-dan-masjid-salman-itb-daur-ulang-air-hujan-dan-air-wudhu</t>
+          <t>https://www.cnbcindonesia.com/market/20250930124321-17-671501/sulap-sampah-jadi-energi-bos-danantara-beberkan-manfaatnya</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -586,12 +582,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>InternasionalTrump Mendadak Kirim Pasukan-Serbu Negara Bagian Ini, Pentagon KagetNews16 menit yang lalu</t>
+          <t>Bos Danantara Ungkap Investasi Proyek Sampah Jadi Energi Rp2,3 TriliunMarket18 menit yang lalu</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -601,7 +597,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929112109-4-671019/trump-mendadak-kirim-pasukan-serbu-negara-bagian-ini-pentagon-kaget</t>
+          <t>https://www.cnbcindonesia.com/market/20250930132253-17-671529/bos-danantara-ungkap-investasi-proyek-sampah-jadi-energi-rp23-triliun</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -609,12 +605,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Dongkrak Talenta Catur, Telkomsel Umumkan Pemenang Chessnation 2025Lifestyle22 menit yang lalu</t>
+          <t>Dikuasai Asing! 11 Emiten Raksasa RI Ini Dikendalikan Jepang &amp; AmerikaResearch24 menit yang lalu</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -624,7 +620,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/lifestyle/20250929131324-33-671086/dongkrak-talenta-catur-telkomsel-umumkan-pemenang-chessnation-2025</t>
+          <t>https://www.cnbcindonesia.com/research/20250930093727-128-671385/dikuasai-asing-11-emiten-raksasa-ri-ini-dikendalikan-jepang-amerika</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
@@ -632,12 +628,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CNBC InsightMiliarder Pertama Dunia Kirim Uang Bantu RI Basmi Cacingan-Bangun WCEntrepreneur26 menit yang lalu</t>
+          <t>Tanggal Peluncuran iPhone 17 di RI Terungkap, Harga Tembus Rp 42 JutaTech29 menit yang lalu</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -647,7 +643,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/entrepreneur/20230929083409-25-476380/miliarder-pertama-dunia-kirim-uang-bantu-ri-basmi-cacingan-bangun-wc</t>
+          <t>https://www.cnbcindonesia.com/tech/20250930125540-37-671520/tanggal-peluncuran-iphone-17-di-ri-terungkap-harga-tembus-rp-42-juta</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -655,12 +651,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Contact Center Pegadaian Borong Penghargaan di Ajang ICCA 2025News28 menit yang lalu</t>
+          <t>Pendapatan Anjlok, Laba Solusi Bangun (SMCB) Naik 63%! Ini PenyebabnyaMarket33 menit yang lalu</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -670,7 +666,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929125412-4-671079/contact-center-pegadaian-borong-penghargaan-di-ajang-icca-2025</t>
+          <t>https://www.cnbcindonesia.com/market/20250930112331-17-671452/pendapatan-anjlok-laba-solusi-bangun--smcb--naik-63-ini-penyebabnya</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -678,12 +674,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Kebakaran Data Center Hancur Dilahap Api, Layanan Publik Lumpuh TotalTech31 menit yang lalu</t>
+          <t>Bukan Keluarga Raja, Ini Orang Terkaya di Dubai Berharta Rp 285 TLifestyle38 menit yang lalu</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -693,7 +689,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250929121850-37-671058/kebakaran-data-center-hancur-dilahap-api-layanan-publik-lumpuh-total</t>
+          <t>https://www.cnbcindonesia.com/lifestyle/20250930110544-33-671444/bukan-keluarga-raja-ini-orang-terkaya-di-dubai-berharta-rp-285-t</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -701,12 +697,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>INET Umumkan Rights Issue, Incar Dana Segar Rp3,2 TriliunMarket36 menit yang lalu</t>
+          <t>Purbaya Janji Lunasi Tunggakan ke BUMN Rp55 T: Tapi Jangan Rugi Terus!News43 menit yang lalu</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -716,20 +712,24 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250929112514-17-671018/inet-umumkan-rights-issue-incar-dana-segar-rp32-triliun</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/news/20250930125556-4-671517/purbaya-janji-lunasi-tunggakan-ke-bumn-rp55-t-tapi-jangan-rugi-terus</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>purbaya</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Prabowo: Aku Tuh Terus Terang Aja Lho, Saya Nggak Dendam sama AniesNews38 menit yang lalu</t>
+          <t>InternasionalIni Reaksi Hamas soal Deal Trump-Netanyahu, Perang Gaza Kelar?News44 menit yang lalu</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -739,24 +739,20 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929130421-4-671083/prabowo-aku-tuh-terus-terang-aja-lho-saya-nggak-dendam-sama-anies</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>prabowo</t>
-        </is>
-      </c>
+          <t>https://www.cnbcindonesia.com/news/20250930122609-4-671483/ini-reaksi-hamas-soal-deal-trump-netanyahu-perang-gaza-kelar</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Daebak! V BTS Dinobatkan Jadi Pria Paling Tampan di Dunia 2025Lifestyle41 menit yang lalu</t>
+          <t>Kapan Program Magang Digaji Rp3,3 Juta Dimulai? Begini Kata MenakerNews45 menit yang lalu</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -766,7 +762,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/lifestyle/20250929120602-33-671059/daebak-v-bts-dinobatkan-jadi-pria-paling-tampan-di-dunia-2025</t>
+          <t>https://www.cnbcindonesia.com/news/20250930125516-4-671519/kapan-program-magang-digaji-rp33-juta-dimulai-begini-kata-menaker</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
@@ -774,12 +770,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Zulhas Cs Mau Kebut Kawasan Pangan Wanam, Ada Pengembangan Etanol-B50News42 menit yang lalu</t>
+          <t>TASPEN Lakukan Ini Buat Perkuat Transparansi &amp; Efektivitas PengawasanNews49 menit yang lalu</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -789,7 +785,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929123411-4-671063/zulhas-cs-mau-kebut-kawasan-pangan-wanam-ada-pengembangan-etanol-b50</t>
+          <t>https://www.cnbcindonesia.com/news/20250930125507-4-671518/taspen-lakukan-ini-buat-perkuat-transparansi-efektivitas-pengawasan</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
@@ -797,12 +793,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Prabowo Klaim Usai Hapus 145 Aturan Soal Pupuk, ada yang PeringatkanNews44 menit yang lalu</t>
+          <t>InternasionalRamai Perusahaan Jepang 'Buru' Pekerja WNI, Ini AlasannyaNews54 menit yang lalu</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -812,24 +808,20 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929124914-4-671077/prabowo-klaim-usai-hapus-145-aturan-soal-pupuk-ada-yang-peringatkan</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>prabowo</t>
-        </is>
-      </c>
+          <t>https://www.cnbcindonesia.com/news/20250930122336-4-671481/ramai-perusahaan-jepang-buru-pekerja-wni-ini-alasannya</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Live Now! BPRS Buka-Bukaan Peluang dan Tantangan Ekonomi Syariah RINews46 menit yang lalu</t>
+          <t>Bumi Kedatangan Komet Raksasa Oktober 2025, Ini Penjelasan IlmuwanTech1 jam yang lalu</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -839,7 +831,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929120632-4-671040/live-now-bprs-buka-bukaan-peluang-dan-tantangan-ekonomi-syariah-ri</t>
+          <t>https://www.cnbcindonesia.com/tech/20250930110920-37-671443/bumi-kedatangan-komet-raksasa-oktober-2025-ini-penjelasan-ilmuwan</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
@@ -847,12 +839,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Baru Berlaku 2023, Kok UU P2SK Direvisi Lagi? Begini Penjelasannya!News50 menit yang lalu</t>
+          <t>Airlangga Hartarto Datangi Langsung Menaker di Kantornya, Ada Apa?News1 jam yang lalu</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -862,7 +854,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929102816-4-670987/baru-berlaku-2023-kok-uu-p2sk-direvisi-lagi-begini-penjelasannya</t>
+          <t>https://www.cnbcindonesia.com/news/20250930124008-4-671499/airlangga-hartarto-datangi-langsung-menaker-di-kantornya-ada-apa</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -870,12 +862,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Cerita Mamimu, Dari Dapur Rumah Hingga Perluas Pasar Berkat TASPENNews55 menit yang lalu</t>
+          <t>Erick Thohir Bantah Tuduhan Mengintervensi FIFA atas Sanksi MalaysiaLifestyle1 jam yang lalu</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -885,7 +877,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929124209-4-671070/cerita-mamimu-dari-dapur-rumah-hingga-perluas-pasar-berkat-taspen</t>
+          <t>https://www.cnbcindonesia.com/lifestyle/20250930111515-33-671459/erick-thohir-bantah-tuduhan-mengintervensi-fifa-atas-sanksi-malaysia</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
@@ -893,12 +885,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Terungkap! Sepatu Impor KW Nike Cs di Senen-Jatinegara dari Negara IniNews56 menit yang lalu</t>
+          <t>Shutdown Jadi Hantu Abadi Ekonomi AS: Puluhan Presiden Jadi KorbanResearch1 jam yang lalu</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -908,7 +900,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929111144-4-671008/terungkap-sepatu-impor-kw-nike-cs-di-senen-jatinegara-dari-negara-ini</t>
+          <t>https://www.cnbcindonesia.com/research/20250930103308-128-671425/shutdown-jadi-hantu-abadi-ekonomi-as-puluhan-presiden-jadi-korban</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
@@ -916,12 +908,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Cara Cek Bansos Rp 600 Ribu Pakai KTP, Oktober Mulai CairTech59 menit yang lalu</t>
+          <t>IHSG Turun 0,33%, Tiga Saham Diburu Saat Emiten Bank Jumbo RontokMarket1 jam yang lalu</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -931,7 +923,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250929123352-37-671069/cara-cek-bansos-rp-600-ribu-pakai-ktp-oktober-mulai-cair</t>
+          <t>https://www.cnbcindonesia.com/market/20250930120706-17-671485/ihsg-turun-033-tiga-saham-diburu-saat-emiten-bank-jumbo-rontok</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
@@ -939,12 +931,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Diburu Interpol, Ini Profil Duo Buron Kasus Keuangan RI Paling DicariMarket1 jam yang lalu</t>
+          <t>Sudah Direstrukturisasi, Krakatau Steel Masih Punya Utang Rp 28,37 TMarket1 jam yang lalu</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -954,7 +946,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250929110315-17-671004/diburu-interpol-ini-profil-duo-buron-kasus-keuangan-ri-paling-dicari</t>
+          <t>https://www.cnbcindonesia.com/market/20250930105211-17-671442/sudah-direstrukturisasi-krakatau-steel-masih-punya-utang-rp-2837-t</t>
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
@@ -962,12 +954,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Prabowo Umumkan Akan Segera Bangun Tanggul Laut Raksasa di PanturaNews1 jam yang lalu</t>
+          <t>Buruh Batalkan Aksi Demo Hari Ini ke DPR, Terungkap AlasannyaNews1 jam yang lalu</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -977,24 +969,20 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929123959-4-671067/prabowo-umumkan-akan-segera-bangun-tanggul-laut-raksasa-di-pantura</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>prabowo</t>
-        </is>
-      </c>
+          <t>https://www.cnbcindonesia.com/news/20250930122350-4-671482/buruh-batalkan-aksi-demo-hari-ini-ke-dpr-terungkap-alasannya</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>5 Bahaya HP Jarang Update iOS di iPhone dan OS di AndroidTech1 jam yang lalu</t>
+          <t>Purbaya: Sebulan Subsidi &amp; Kompensasi BUMN Tak Dibayar, Dirjen GantiNews1 jam yang lalu</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1004,20 +992,24 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250929111544-37-671012/5-bahaya-hp-jarang-update-ios-di-iphone-dan-os-di-android</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/news/20250930120753-4-671469/purbaya-sebulan-subsidi-kompensasi-bumn-tak-dibayar-dirjen-ganti</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>purbaya</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Saham PGUN Haji Isam OTW Jadi Raja Konsumer RI, HMSP-UNVR-AMRT LewatMarket1 jam yang lalu</t>
+          <t>Bos Badan Pangan Ingatkan Beras Busuk Tak Boleh Diedarkan, Stok Aman?News1 jam yang lalu</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1027,7 +1019,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250929105938-17-671000/saham-pgun-haji-isam-otw-jadi-raja-konsumer-ri-hmsp-unvr-amrt-lewat</t>
+          <t>https://www.cnbcindonesia.com/news/20250930111012-4-671445/bos-badan-pangan-ingatkan-beras-busuk-tak-boleh-diedarkan-stok-aman</t>
         </is>
       </c>
       <c r="E25" t="inlineStr"/>
@@ -1035,12 +1027,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Ekspor RI ke UE-Kanada Bakal Melejit 2 Kali Lipat, Ini PemicunyaNews1 jam yang lalu</t>
+          <t>Ekosistem Baterai UV Ubah Paradigma Ekonomi IndonesiaOpini1 jam yang lalu</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1050,7 +1042,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929115812-4-671039/ekspor-ri-ke-ue-kanada-bakal-melejit-2-kali-lipat-ini-pemicunya</t>
+          <t>https://www.cnbcindonesia.com/opini/20250930103621-14-671429/ekosistem-baterai-uv-ubah-paradigma-ekonomi-indonesia</t>
         </is>
       </c>
       <c r="E26" t="inlineStr"/>
@@ -1058,12 +1050,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Studi Ungkap 13 Ciri Psikopat yang Bisa Dikenali sebelum DewasaLifestyle1 jam yang lalu</t>
+          <t>Soal Subsidi 2024, Purbaya: Jika Ada yang Belum Dibayar Hadap Saya!News1 jam yang lalu</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1073,20 +1065,24 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/lifestyle/20250929111337-33-671010/studi-ungkap-13-ciri-psikopat-yang-bisa-dikenali-sebelum-dewasa</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/news/20250930120705-4-671468/soal-subsidi-2024-purbaya-jika-ada-yang-belum-dibayar-hadap-saya</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>purbaya</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>IHSG Sesi I Naik 0,6%,Market Cap Tembus Rp 15.000 TriliunMarket1 jam yang lalu</t>
+          <t>NASA Temukan Tanda Kehidupan Paling Jelas di Mars, Cek FaktanyaTech1 jam yang lalu</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1096,7 +1092,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250929114719-17-671029/ihsg-sesi-i-naik-06market-cap-tembus-rp-15000-triliun</t>
+          <t>https://www.cnbcindonesia.com/tech/20250930104626-37-671437/nasa-temukan-tanda-kehidupan-paling-jelas-di-mars-cek-faktanya</t>
         </is>
       </c>
       <c r="E28" t="inlineStr"/>
@@ -1104,12 +1100,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Avanza-Veloz Hybrid Bakal Hadir di RI? Ini Bocoran dari ToyotaNews1 jam yang lalu</t>
+          <t>Terungkap! Bandung Bakal Punya KRL, Rutenya IniNews1 jam yang lalu</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1119,7 +1115,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929111022-4-671007/avanza-veloz-hybrid-bakal-hadir-di-ri-ini-bocoran-dari-toyota</t>
+          <t>https://www.cnbcindonesia.com/news/20250930115522-4-671466/terungkap-bandung-bakal-punya-krl-rutenya-ini</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
@@ -1127,12 +1123,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2 dari 3 Petani RI Berusia Tua, Siapa yang Menanam Padi?Research1 jam yang lalu</t>
+          <t>Bos Danantara Blak-Blakan Soal Merger Asuransi BUMN, IFG Jadi HoldingMarket1 jam yang lalu</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1142,7 +1138,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/research/20250926150159-128-670516/2-dari-3-petani-ri-berusia-tua-siapa-yang-menanam-padi</t>
+          <t>https://www.cnbcindonesia.com/market/20250930115445-17-671467/bos-danantara-blak-blakan-soal-merger-asuransi-bumn-ifg-jadi-holding</t>
         </is>
       </c>
       <c r="E30" t="inlineStr"/>
@@ -1150,12 +1146,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Purbaya Terima Kritik Rocky Gerung, Tapi Harus Minta Maaf Kalau SalahNews1 jam yang lalu</t>
+          <t>InternasionalPerang Dagang Lagi! Trump Umumkan Tarif Baru, 25%-50% Mulai 14 OktoberNews1 jam yang lalu</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1165,24 +1161,20 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929114309-4-671027/purbaya-terima-kritik-rocky-gerung-tapi-harus-minta-maaf-kalau-salah</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>purbaya</t>
-        </is>
-      </c>
+          <t>https://www.cnbcindonesia.com/news/20250930115046-4-671465/perang-dagang-lagi-trump-umumkan-tarif-baru-25-50-mulai-14-oktober</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Raksasa Tekstil di Bandung Pailit, Sudah Setop Operasi Sejak 2024Market1 jam yang lalu</t>
+          <t>Purbaya Ungkap Harga Sebenarnya Pertalite, Solar Sampai LPGNews1 jam yang lalu</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1192,20 +1184,24 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250929120928-17-671044/raksasa-tekstil-di-bandung-pailit-sudah-setop-operasi-sejak-2024</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/news/20250930112226-4-671449/purbaya-ungkap-harga-sebenarnya-pertalite-solar-sampai-lpg</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>purbaya</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Prabowo Ungkap ada 'Harta Karun' Dibalik Limbah TimahNews1 jam yang lalu</t>
+          <t>InternasionalPMI Manufaktur China Kontraksi, Enam Kali Berturut-turutNews1 jam yang lalu</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1215,24 +1211,20 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929114953-4-671031/prabowo-ungkap-ada-harta-karun-dibalik-limbah-timah</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>prabowo</t>
-        </is>
-      </c>
+          <t>https://www.cnbcindonesia.com/news/20250930113331-4-671455/pmi-manufaktur-china-kontraksi-enam-kali-berturut-turut</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Lebih dari 100 Lapangan Padel Bangkrut, Dulu Viral sekarang SuramLifestyle1 jam yang lalu</t>
+          <t>BUMN Jangan Khawatir, Purbaya Siap Bayar Subsidi Oktober 2025News1 jam yang lalu</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1242,20 +1234,24 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/lifestyle/20250929105342-33-670996/lebih-dari-100-lapangan-padel-bangkrut-dulu-viral-sekarang-suram</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/news/20250930114552-4-671458/bumn-jangan-khawatir-purbaya-siap-bayar-subsidi-oktober-2025</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>purbaya</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>InternasionalPetaka Hantam Tetangga RI, Bandara Ditutup-Ribuan Orang DievakuasiNews1 jam yang lalu</t>
+          <t>Rupiah Perkasa Lawan Dolar, Ekonom Ungkap Penyebab UtamanyaNews1 jam yang lalu</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1265,7 +1261,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929113831-4-671021/petaka-hantam-tetangga-ri-bandara-ditutup-ribuan-orang-dievakuasi</t>
+          <t>https://www.cnbcindonesia.com/news/20250930114126-4-671457/rupiah-perkasa-lawan-dolar-ekonom-ungkap-penyebab-utamanya</t>
         </is>
       </c>
       <c r="E35" t="inlineStr"/>
@@ -1273,12 +1269,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Prabowo ke PKS: 2 Kali Dukung 2 Kali Kalah, Giliran Menang Gak DukungNews1 jam yang lalu</t>
+          <t>6 Alasan Kenapa Harga Emas Bisa Meledak ke LangitResearch1 jam yang lalu</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1288,24 +1284,20 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929115030-4-671041/prabowo-ke-pks-2-kali-dukung-2-kali-kalah-giliran-menang-gak-dukung</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>prabowo</t>
-        </is>
-      </c>
+          <t>https://www.cnbcindonesia.com/research/20250930104459-128-671436/6-alasan-kenapa-harga-emas-bisa-meledak-ke-langit</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Telkom, Telkomsel, Indosat, XLSmart Pilih Dian Siswarini Ketua ATSITech1 jam yang lalu</t>
+          <t>Green Era Energy Kembali Jual Saham BREN, Kali Ini Raup Rp698 MiliarMarket2 jam yang lalu</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1315,7 +1307,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250929113231-37-671024/telkom-telkomsel-indosat-xlsmart-pilih-dian-siswarini-ketua-atsi</t>
+          <t>https://www.cnbcindonesia.com/market/20250930091033-17-671374/green-era-energy-kembali-jual-saham-bren-kali-ini-raup-rp698-miliar</t>
         </is>
       </c>
       <c r="E37" t="inlineStr"/>
@@ -1323,12 +1315,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>MMIX Bakal Bagikan Saham Bonus 1:1 Cek Jadwalnya!Market1 jam yang lalu</t>
+          <t>Pengusaha Baja Teriak, RI Lemah Lawan Serbuan Barang Impor &amp; DumpingNews2 jam yang lalu</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1338,7 +1330,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250929115719-17-671038/mmix-bakal-bagikan-saham-bonus-11-cek-jadwalnya</t>
+          <t>https://www.cnbcindonesia.com/news/20250930103725-4-671431/pengusaha-baja-teriak-ri-lemah-lawan-serbuan-barang-impor-dumping</t>
         </is>
       </c>
       <c r="E38" t="inlineStr"/>
@@ -1346,12 +1338,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Sepatu Impor Nike Cs di Senen-Jatinegara Barang KW-Harga di Luar NalarNews1 jam yang lalu</t>
+          <t>Pasien Alzheimer Termuda Dunia Baru 19 Tahun, Ahli Saraf BingungLifestyle2 jam yang lalu</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1361,7 +1353,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929105022-4-670995/sepatu-impor-nike-cs-di-senen-jatinegara-barang-kw-harga-di-luar-nalar</t>
+          <t>https://www.cnbcindonesia.com/lifestyle/20250930104202-33-671434/pasien-alzheimer-termuda-dunia-baru-19-tahun-ahli-saraf-bingung</t>
         </is>
       </c>
       <c r="E39" t="inlineStr"/>
@@ -1369,12 +1361,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>InternasionalPutin Menggila! Rusia Tembak 595 Drone 'Bakar' Kyiv, Jet NATO TurunNews1 jam yang lalu</t>
+          <t>Ada Transaksi Jumbo di MMLP, Astra Resmi Jadi Pengendali Baru?Market2 jam yang lalu</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1384,7 +1376,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929111809-4-671013/putin-menggila-rusia-tembak-595-drone-bakar-kyiv-jet-nato-turun</t>
+          <t>https://www.cnbcindonesia.com/market/20250930111133-17-671453/ada-transaksi-jumbo-di-mmlp-astra-resmi-jadi-pengendali-baru</t>
         </is>
       </c>
       <c r="E40" t="inlineStr"/>
@@ -1392,12 +1384,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Prabowo Ungkit Rusuh 29 Agustus: Ada Keterlibatan Kekuatan TertentuNews1 jam yang lalu</t>
+          <t>Pesawat Diserang Maling, Nasib Penumpang MemprihatinkanTech2 jam yang lalu</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1407,24 +1399,20 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929114729-4-671030/prabowo-ungkit-rusuh-29-agustus-ada-keterlibatan-kekuatan-tertentu</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>prabowo</t>
-        </is>
-      </c>
+          <t>https://www.cnbcindonesia.com/tech/20250930103605-37-671428/pesawat-diserang-maling-nasib-penumpang-memprihatinkan</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>DAIKIN Resmikan Pusat Keunggulan Pertama di BekasiNews1 jam yang lalu</t>
+          <t>BULL Private Placement Rp254 Miliar, Investor Hong Kong Jadi PemborongMarket2 jam yang lalu</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1434,7 +1422,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929114311-4-671028/daikin-resmikan-pusat-keunggulan-pertama-di-bekasi</t>
+          <t>https://www.cnbcindonesia.com/market/20250930100439-17-671417/bull-private-placement-rp254-miliar-investor-hong-kong-jadi-pemborong</t>
         </is>
       </c>
       <c r="E42" t="inlineStr"/>
@@ -1442,12 +1430,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Penutupan Munas VI PKSPrabowo Lapor Penerima MBG Dekati 30 Juta, Akui ada Keracunan MakananNews1 jam yang lalu</t>
+          <t>Purbaya Lapor ke DPR, Subsidi BBM Cs 2025 Tembus Rp479 TNews2 jam yang lalu</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1457,24 +1445,24 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929100637-4-670965/prabowo-lapor-penerima-mbg-dekati-30-juta-akui-ada-keracunan-makanan</t>
+          <t>https://www.cnbcindonesia.com/news/20250930111917-4-671448/purbaya-lapor-ke-dpr-subsidi-bbm-cs-2025-tembus-rp479-t</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>mbg</t>
+          <t>purbaya</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Harga Minyak Tergelincir Awal Pekan, Brent Kembali ke Bawah US$70Market1 jam yang lalu</t>
+          <t>Purbaya Pede Investor Asing Bakal Serbu RI: Mereka Bakal Menikmati!Market2 jam yang lalu</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1484,20 +1472,24 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250929102957-17-670983/harga-minyak-tergelincir-awal-pekan-brent-kembali-ke-bawah-us-70</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/market/20250930090917-17-671370/purbaya-pede-investor-asing-bakal-serbu-ri-mereka-bakal-menikmati</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>purbaya</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Rupiah Anjlok 20% vs Real Arab, Umroh Bawa Rp 10 Juta Langsung MiskinResearch2 jam yang lalu</t>
+          <t>Bukan Surabaya, Kereta Cepat RI Ternyata Dirancang Tembus Sampai SiniNews2 jam yang lalu</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1507,7 +1499,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/research/20250929102709-128-670989/rupiah-anjlok-20-vs-real-arab-umroh-bawa-rp-10-juta-langsung-miskin</t>
+          <t>https://www.cnbcindonesia.com/news/20250930111016-4-671446/bukan-surabaya-kereta-cepat-ri-ternyata-dirancang-tembus-sampai-sini</t>
         </is>
       </c>
       <c r="E45" t="inlineStr"/>
@@ -1515,12 +1507,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Prabowo Titahkan TNI-Polri Operasi Besar-Besaran di Babel, Ada Apa?News2 jam yang lalu</t>
+          <t>Cukai Rokok Tak Naik, Wamenperin: Perusahaan Cuma Menikmati 20%News2 jam yang lalu</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1530,24 +1522,24 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929113914-4-671023/prabowo-titahkan-tni-polri-operasi-besar-besaran-di-babel-ada-apa</t>
+          <t>https://www.cnbcindonesia.com/news/20250930102534-4-671423/cukai-rokok-tak-naik-wamenperin-perusahaan-cuma-menikmati-20</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>prabowo</t>
+          <t>cukai</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Pengumuman! Bakal Ada Sistem Baru, Ekspor Bakal Makin MudahNews2 jam yang lalu</t>
+          <t>Sillicon Valley Connection Jual 10 Juta Saham WGSH, Nilainya TerungkapMarket2 jam yang lalu</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1557,7 +1549,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929112225-4-671014/pengumuman-bakal-ada-sistem-baru-ekspor-bakal-makin-mudah</t>
+          <t>https://www.cnbcindonesia.com/market/20250930101106-17-671419/sillicon-valley-connection-jual-10-juta-saham-wgsh-nilainya-terungkap</t>
         </is>
       </c>
       <c r="E47" t="inlineStr"/>
@@ -1565,12 +1557,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Jelang Merger dengan ADMF, Bursa Gembok Saham MFINMarket2 jam yang lalu</t>
+          <t>Bos Antam Beberkan Susahnya Dapat Pasokan Emas dari Tambang RINews2 jam yang lalu</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1580,7 +1572,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250929083437-17-670930/jelang-merger-dengan-admf-bursa-gembok-saham-mfin</t>
+          <t>https://www.cnbcindonesia.com/news/20250930103114-4-671430/bos-antam-beberkan-susahnya-dapat-pasokan-emas-dari-tambang-ri</t>
         </is>
       </c>
       <c r="E48" t="inlineStr"/>
@@ -1588,12 +1580,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Dibongkar Prabowo! 80% Produksi Timah RI Ternyata DiselundupkanNews2 jam yang lalu</t>
+          <t>Purbaya Bertandang ke DPR, Lapor Realisasi Subsidi &amp; KompensasiNews2 jam yang lalu</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1603,24 +1595,24 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929113128-4-671020/dibongkar-prabowo-80-produksi-timah-ri-ternyata-diselundupkan</t>
+          <t>https://www.cnbcindonesia.com/news/20250930105425-4-671441/purbaya-bertandang-ke-dpr-lapor-realisasi-subsidi-kompensasi</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>prabowo</t>
+          <t>purbaya</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Penutupan Munas VI PKSPrabowo Geram Korupsi di RI Parah: Orang Pintar itu Sering Nyolong!News2 jam yang lalu</t>
+          <t>Internet Diblokir Total, Penerbangan Batal-Negara Gelap GulitaTech2 jam yang lalu</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1630,7 +1622,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929100720-4-670966/prabowo-geram-korupsi-di-ri-parah-orang-pintar-itu-sering-nyolong</t>
+          <t>https://www.cnbcindonesia.com/tech/20250930101257-37-671418/internet-diblokir-total-penerbangan-batal-negara-gelap-gulita</t>
         </is>
       </c>
       <c r="E50" t="inlineStr"/>
@@ -1638,12 +1630,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Waspada Angin Kencang Hantam Jakarta, Cek Peringatan Baru BMKGTech2 jam yang lalu</t>
+          <t>Bos Danantara Ungkap RI Darurat Sampah, Jumlahnya 16.500 Lapangan BolaMarket2 jam yang lalu</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1653,7 +1645,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250929105759-37-670998/waspada-angin-kencang-hantam-jakarta-cek-peringatan-baru-bmkg</t>
+          <t>https://www.cnbcindonesia.com/market/20250930104814-17-671440/bos-danantara-ungkap-ri-darurat-sampah-jumlahnya-16500-lapangan-bola</t>
         </is>
       </c>
       <c r="E51" t="inlineStr"/>
@@ -1661,12 +1653,12 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Prabowo: Sebagian Besar Rakyat Kita Belum Menikmati Kekayaan IndonesiaNews2 jam yang lalu</t>
+          <t>Komisi XI DPR Buka-bukaan Soal Proses Pembahasan RUU P2SK, Simak!News2 jam yang lalu</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1676,24 +1668,20 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929112012-4-671017/prabowo-sebagian-besar-rakyat-kita-belum-menikmati-kekayaan-indonesia</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>prabowo</t>
-        </is>
-      </c>
+          <t>https://www.cnbcindonesia.com/news/20250930101809-4-671420/komisi-xi-dpr-buka-bukaan-soal-proses-pembahasan-ruu-p2sk-simak</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Prabowo Sebut Ada 1.000 Tambang Timah Ilegal di Bangka BelitungNews2 jam yang lalu</t>
+          <t>MIND ID Perkuat Kinerja Lewat Inovasi Hilirisasi MineralNews3 jam yang lalu</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1703,24 +1691,20 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929102429-4-671015/prabowo-sebut-ada-1000-tambang-timah-ilegal-di-bangka-belitung</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>prabowo</t>
-        </is>
-      </c>
+          <t>https://www.cnbcindonesia.com/news/20250930104358-4-671435/mind-id-perkuat-kinerja-lewat-inovasi-hilirisasi-mineral</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>14 Makanan Sehari-Hari yang Mengandung Mikroplastik, Ada Favorit Kamu?Lifestyle2 jam yang lalu</t>
+          <t>Pasar Kelebihan Pasokan, Harga Minyak Dunia AnjlokMarket3 jam yang lalu</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1730,7 +1714,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/lifestyle/20250929103251-33-670986/14-makanan-sehari-hari-yang-mengandung-mikroplastik-ada-favorit-kamu</t>
+          <t>https://www.cnbcindonesia.com/market/20250930094657-17-671393/pasar-kelebihan-pasokan-harga-minyak-dunia-anjlok</t>
         </is>
       </c>
       <c r="E54" t="inlineStr"/>
@@ -1738,12 +1722,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Wah! Purbaya Tiba-tiba Sidak Kantor BNINews2 jam yang lalu</t>
+          <t>Duel Sengit: RI vs Malaysia Saling Tikung Akuisisi Emiten RaksasaResearch3 jam yang lalu</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1753,24 +1737,20 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929110139-4-671001/wah-purbaya-tiba-tiba-sidak-kantor-bni</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>purbaya</t>
-        </is>
-      </c>
+          <t>https://www.cnbcindonesia.com/research/20250930093928-128-671387/duel-sengit-ri-vs-malaysia-saling-tikung-akuisisi-emiten-raksasa</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Mundur dari Direktur Bank Permata, Abdy Dharma Pindah ke Bangkok BankMarket2 jam yang lalu</t>
+          <t>3 Emiten Teknologi Mau Rights Issue, Galang Dana Lebih dari Rp 9 TMarket3 jam yang lalu</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1780,7 +1760,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250929091636-17-670956/mundur-dari-direktur-bank-permata-abdy-dharma-pindah-ke-bangkok-bank</t>
+          <t>https://www.cnbcindonesia.com/market/20250930093044-17-671386/3-emiten-teknologi-mau-rights-issue-galang-dana-lebih-dari-rp-9-t</t>
         </is>
       </c>
       <c r="E56" t="inlineStr"/>
@@ -1788,12 +1768,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>InternasionalTerima Duit Suap Rp 626 M, Eks Mentan Dihukum Mati di SiniNews2 jam yang lalu</t>
+          <t>InternasionalNetanyahu Tiba-Tiba Minta Maaf ke Pemimpin Arab, Janji Tak Ulangi LagiNews3 jam yang lalu</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1803,7 +1783,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929103511-4-670988/terima-duit-suap-rp-626-m-eks-mentan-dihukum-mati-di-sini</t>
+          <t>https://www.cnbcindonesia.com/news/20250930102040-4-671422/netanyahu-tiba-tiba-minta-maaf-ke-pemimpin-arab-janji-tak-ulangi-lagi</t>
         </is>
       </c>
       <c r="E57" t="inlineStr"/>
@@ -1811,12 +1791,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Penutupan Munas VI PKSKelakar Prabowo: PKS Gabung Usai Merantau, Usul Prof ITB Jadi MenteriNews2 jam yang lalu</t>
+          <t>Janji Prabowo Bisa Selamatkan Uang Negara Rp 67 Triliun, Ini SumbernyaNews3 jam yang lalu</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1826,24 +1806,20 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929110348-4-671003/kelakar-prabowo-pks-gabung-usai-merantau-usul-prof-itb-jadi-menteri</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>prabowo</t>
-        </is>
-      </c>
+          <t>https://www.cnbcindonesia.com/news/20250930102537-4-671424/janji-prabowo-bisa-selamatkan-uang-negara-rp-67-triliun-ini-sumbernya</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>BI Luncurkan Matchmaking Overnight Index Swap, Ini TujuannyaNews2 jam yang lalu</t>
+          <t>Ikut Kata Prabowo, Bulog Mau Bangun 100 Gudang-Ini LokasinyaNews3 jam yang lalu</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1853,7 +1829,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929105725-4-670997/bi-luncurkan-matchmaking-overnight-index-swap-ini-tujuannya</t>
+          <t>https://www.cnbcindonesia.com/news/20250930101835-4-671421/ikut-kata-prabowo-bulog-mau-bangun-100-gudang-ini-lokasinya</t>
         </is>
       </c>
       <c r="E59" t="inlineStr"/>
@@ -1861,12 +1837,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Dunia Makin Menyeramkan, Prabowo Ungkap Ketakutan Besar Eropa!News2 jam yang lalu</t>
+          <t>Purbaya Ramal Ekonomi Kuartal IV-2025 di Atas 5,5%News3 jam yang lalu</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1876,24 +1852,24 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929110147-4-671002/dunia-makin-menyeramkan-prabowo-ungkap-ketakutan-besar-eropa</t>
+          <t>https://www.cnbcindonesia.com/news/20250930094808-4-671395/purbaya-ramal-ekonomi-kuartal-iv-2025-di-atas-55</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>prabowo</t>
+          <t>purbaya</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Memahami Ragam Sistem Pendidikan Global, Studi Kasus Gibran RakabumingOpini2 jam yang lalu</t>
+          <t>Arab Beli Pencipta Game FIFA Rp 917 Triliun, Menantu Trump PatunganTech3 jam yang lalu</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1903,7 +1879,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/opini/20250929094358-14-670959/memahami-ragam-sistem-pendidikan-global-studi-kasus-gibran-rakabuming</t>
+          <t>https://www.cnbcindonesia.com/tech/20250930082722-37-671359/arab-beli-pencipta-game-fifa-rp-917-triliun-menantu-trump-patungan</t>
         </is>
       </c>
       <c r="E61" t="inlineStr"/>
@@ -1911,12 +1887,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>InternasionalMedia Asing Tiba-Tiba Sorot Bali, Sebut Jadi KorbanNews2 jam yang lalu</t>
+          <t>Selama Ini Terbuang Sia-Sia, Limbah Timah Bernilai Fantastis!News3 jam yang lalu</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1926,7 +1902,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929102035-4-670968/media-asing-tiba-tiba-sorot-bali-sebut-jadi-korban</t>
+          <t>https://www.cnbcindonesia.com/news/20250930092943-4-671379/selama-ini-terbuang-sia-sia-limbah-timah-bernilai-fantastis</t>
         </is>
       </c>
       <c r="E62" t="inlineStr"/>
@@ -1934,12 +1910,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Wismilak Inti Makmur (WIIM) Bakal Lepas 24 Juta Saham TreasuriMarket2 jam yang lalu</t>
+          <t>Harga Saham Naik Ratusan Persen, BEI Gembok 7 Emiten SekaligusMarket3 jam yang lalu</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1949,7 +1925,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250929093056-17-670957/wismilak-inti-makmur--wiim--bakal-lepas-24-juta-saham-treasuri</t>
+          <t>https://www.cnbcindonesia.com/market/20250930090711-17-671372/harga-saham-naik-ratusan-persen-bei-gembok-7-emiten-sekaligus</t>
         </is>
       </c>
       <c r="E63" t="inlineStr"/>
@@ -1957,12 +1933,12 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Penutupan Munas VI PKSPrabowo Tutup Munas VI PKS: Angka 8 itu Selalu Hadir di Hidup SayaNews2 jam yang lalu</t>
+          <t>6 Profesi Paling Tidak Dipercaya Masyarakat Menurut SurveiLifestyle3 jam yang lalu</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -1972,7 +1948,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929100526-4-670964/prabowo-tutup-munas-vi-pks-angka-8-itu-selalu-hadir-di-hidup-saya</t>
+          <t>https://www.cnbcindonesia.com/lifestyle/20250930085746-33-671367/6-profesi-paling-tidak-dipercaya-masyarakat-menurut-survei</t>
         </is>
       </c>
       <c r="E64" t="inlineStr"/>
@@ -1980,12 +1956,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Robot Tesla Pembawa Maut, Manusia Hampir MeninggalTech2 jam yang lalu</t>
+          <t>InternasionalTetangga RI 'Macan Asia' Terancam Resesi, Bakal Kena di 2040News3 jam yang lalu</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1995,7 +1971,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250929101735-37-670967/robot-tesla-pembawa-maut-manusia-hampir-meninggal</t>
+          <t>https://www.cnbcindonesia.com/news/20250930095211-4-671402/tetangga-ri-macan-asia-terancam-resesi-bakal-kena-di-2040</t>
         </is>
       </c>
       <c r="E65" t="inlineStr"/>
@@ -2003,12 +1979,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Terungkap Jenis Bakteri 'Biang Kerok' Keracunan MBG di Bandung BaratLifestyle3 jam yang lalu</t>
+          <t>Danantara Bahas Proyek Sampah Jadi Energi, Ray Dalio Terlihat HadirMarket3 jam yang lalu</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2018,24 +1994,20 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/lifestyle/20250929095828-33-670962/terungkap-jenis-bakteri-biang-kerok-keracunan-mbg-di-bandung-barat</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>mbg</t>
-        </is>
-      </c>
+          <t>https://www.cnbcindonesia.com/market/20250930094539-17-671392/danantara-bahas-proyek-sampah-jadi-energi-ray-dalio-terlihat-hadir</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>RI Punya Harta Karun Bernilai Fantastis, Tapi Malah Dibuang!News3 jam yang lalu</t>
+          <t>Pengumuman! Kantor Purbaya Lelang Alat Pijat, Balon Sampai SapiNews3 jam yang lalu</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2045,20 +2017,24 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929095936-4-670963/ri-punya-harta-karun-bernilai-fantastis-tapi-malah-dibuang</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/news/20250930092520-4-671377/pengumuman-kantor-purbaya-lelang-alat-pijat-balon-sampai-sapi</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>purbaya</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6 Gerbang Tol Dalam Kota Ditutup Mulai Hari iniNews3 jam yang lalu</t>
+          <t>Tiba-Tiba Asia Jadi Lautan Merah, Rupiah - Yen Terbakar Dolar ASResearch4 jam yang lalu</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2068,7 +2044,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929102057-4-670984/6-gerbang-tol-dalam-kota-ditutup-mulai-hari-ini</t>
+          <t>https://www.cnbcindonesia.com/research/20250930093808-128-671389/tiba-tiba-asia-jadi-lautan-merah-rupiah--yen-terbakar-dolar-as</t>
         </is>
       </c>
       <c r="E68" t="inlineStr"/>
@@ -2076,12 +2052,12 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Bos EXCL Borong Saham Perusahaan Rp 1,59 MiliarMarket3 jam yang lalu</t>
+          <t>Pemilik Cadangan Top 5 Dunia Tapi RI Masih Impor Emas Besar-besaran!News4 jam yang lalu</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2091,7 +2067,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250929091656-17-670952/bos-excl-borong-saham-perusahaan-rp-159-miliar</t>
+          <t>https://www.cnbcindonesia.com/news/20250930091732-4-671375/pemilik-cadangan-top-5-dunia-tapi-ri-masih-impor-emas-besar-besaran</t>
         </is>
       </c>
       <c r="E69" t="inlineStr"/>
@@ -2099,12 +2075,12 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>United Tractors (UNTR) Bagi Dividen Interim Rp2,05 T, Ini JadwalnyaMarket3 jam yang lalu</t>
+          <t>Taspen Serahkan Uang Pensiun ke Sri Mulyani, Netizen PenasaranTech4 jam yang lalu</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2114,7 +2090,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250929101457-17-670969/united-tractors--untr--bagi-dividen-interim-rp205-t-ini-jadwalnya</t>
+          <t>https://www.cnbcindonesia.com/tech/20250930091955-37-671376/taspen-serahkan-uang-pensiun-ke-sri-mulyani-netizen-penasaran</t>
         </is>
       </c>
       <c r="E70" t="inlineStr"/>
@@ -2122,12 +2098,12 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Bursa Gembok Perdagangan Saham 7 Emiten IniMarket3 jam yang lalu</t>
+          <t>Prabowo Sebut BUMN Rugi Bagi Bonus Brengsek, Mau Kirim KPK &amp; KejaksaanMarket4 jam yang lalu</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2137,7 +2113,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250929095117-17-670960/bursa-gembok-perdagangan-saham-7-emiten-ini</t>
+          <t>https://www.cnbcindonesia.com/market/20250930083834-17-671364/prabowo-sebut-bumn-rugi-bagi-bonus-brengsek-mau-kirim-kpk-kejaksaan</t>
         </is>
       </c>
       <c r="E71" t="inlineStr"/>
@@ -2145,12 +2121,12 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Deretan Emiten "Harta Karun", Anda Bisa Jadi Crazy Rich dalam 10 TahunResearch3 jam yang lalu</t>
+          <t>Purbaya Tunda Pungutan PPh Pedagang Online, Ini Kata EcommerceTech4 jam yang lalu</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2160,20 +2136,24 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/research/20250926130822-128-670465/deretan-emiten-harta-karun-anda-bisa-jadi-crazy-rich-dalam-10-tahun</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/tech/20250930091052-37-671371/purbaya-tunda-pungutan-pph-pedagang-online-ini-kata-ecommerce</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>purbaya</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Alasan Ilmiah Daging Hiu Tak Boleh Dimakan, Bukan Cuma Tinggi MerkuriTech3 jam yang lalu</t>
+          <t>Harga Saham Bergerak Tak Wajar, BEI Pantau Ketat 3 Emiten IniMarket4 jam yang lalu</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2183,7 +2163,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250929095807-37-670961/alasan-ilmiah-daging-hiu-tak-boleh-dimakan-bukan-cuma-tinggi-merkuri</t>
+          <t>https://www.cnbcindonesia.com/market/20250930083358-17-671361/harga-saham-bergerak-tak-wajar-bei-pantau-ketat-3-emiten-ini</t>
         </is>
       </c>
       <c r="E73" t="inlineStr"/>
@@ -2191,12 +2171,12 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Prabowo Mau Pindahkan 9.500 ASN ke IKN hingga 2029, Begini TahapannyaNews3 jam yang lalu</t>
+          <t>Peta Timah ASEAN: Laba Jeblok, TINS Tetap Lebih Gahar vs MSC MalaysiaResearch4 jam yang lalu</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2206,24 +2186,20 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929084917-4-670939/prabowo-mau-pindahkan-9500-asn-ke-ikn-hingga-2029-begini-tahapannya</t>
-        </is>
-      </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>prabowo</t>
-        </is>
-      </c>
+          <t>https://www.cnbcindonesia.com/research/20250929125217-128-671078/peta-timah-asean-laba-jeblok-tins-tetap-lebih-gahar-vs-msc-malaysia</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>12 Buah dan Sayuran 'Kotor' yang Mengandung Pestisida Paling TinggiLifestyle3 jam yang lalu</t>
+          <t>Danantara Adakan Rapat, Bahas Proyek Sampah Jadi EnergiMarket4 jam yang lalu</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2233,7 +2209,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/lifestyle/20250929090606-33-670949/12-buah-dan-sayuran-kotor-yang-mengandung-pestisida-paling-tinggi</t>
+          <t>https://www.cnbcindonesia.com/market/20250930091639-17-671373/danantara-adakan-rapat-bahas-proyek-sampah-jadi-energi</t>
         </is>
       </c>
       <c r="E75" t="inlineStr"/>
@@ -2241,12 +2217,12 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Waskita Karya Infrastruktur Umumkan Jual Anak Usaha Rp179,99 MiliarMarket3 jam yang lalu</t>
+          <t>Skandal Naturalisasi Timnas Malaysia, 7 Pemain Kena Sanksi FIFALifestyle4 jam yang lalu</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2256,7 +2232,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250929084954-17-670947/waskita-karya-infrastruktur-umumkan-jual-anak-usaha-rp17999-miliar</t>
+          <t>https://www.cnbcindonesia.com/lifestyle/20250930085305-33-671366/skandal-naturalisasi-timnas-malaysia-7-pemain-kena-sanksi-fifa</t>
         </is>
       </c>
       <c r="E76" t="inlineStr"/>
@@ -2264,12 +2240,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Interpol Buru Bos WanaArtha &amp; Kresna Group usai Ciduk Adrian GunadiMarket3 jam yang lalu</t>
+          <t>InternasionalIsi Proposal Perdamaian Gaza Trump-Netanyahu, Arab &amp; RI Disebut SetujuNews4 jam yang lalu</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2279,7 +2255,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250929092533-17-670955/interpol-buru-bos-wanaartha-kresna-group-usai-ciduk-adrian-gunadi</t>
+          <t>https://www.cnbcindonesia.com/news/20250930090324-4-671369/isi-proposal-perdamaian-gaza-trump-netanyahu-arab-ri-disebut-setuju</t>
         </is>
       </c>
       <c r="E77" t="inlineStr"/>
@@ -2287,12 +2263,12 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>7 Aplikasi Kamera HP Buat Hasilkan Foto Setara DSLR, Cek DaftarnyaTech4 jam yang lalu</t>
+          <t>Rupiah Kembali Menguat, Dolar AS Dibuka Turun ke Rp16.650Market4 jam yang lalu</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2302,7 +2278,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250929092522-37-670954/7-aplikasi-kamera-hp-buat-hasilkan-foto-setara-dslr-cek-daftarnya</t>
+          <t>https://www.cnbcindonesia.com/market/20250930083512-17-671362/rupiah-kembali-menguat-dolar-as-dibuka-turun-ke-rp16650</t>
         </is>
       </c>
       <c r="E78" t="inlineStr"/>
@@ -2310,12 +2286,12 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Besok, Malaysia Resmi Turunkan Harga BBM RON 95 Jadi Rp7.849 per LiterNews4 jam yang lalu</t>
+          <t>Lanjutkan Reli, IHSG Dibuka Menguat Tipis 0,18% ke 8.137Market4 jam yang lalu</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2325,7 +2301,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929094011-4-670958/besok-malaysia-resmi-turunkan-harga-bbm-ron-95-jadi-rp7849-per-liter</t>
+          <t>https://www.cnbcindonesia.com/market/20250930085009-17-671368/lanjutkan-reli-ihsg-dibuka-menguat-tipis-018-ke-8137</t>
         </is>
       </c>
       <c r="E79" t="inlineStr"/>
@@ -2333,12 +2309,12 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Asia Pukul Balik Amerika: Dolar AS Ditendang, Won - Rupiah Jadi RajaResearch4 jam yang lalu</t>
+          <t>Bukan Cuma Orang Tua, Anak Muda Wajib Waspada Jika Merasa Nyeri DadaLifestyle4 jam yang lalu</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2348,7 +2324,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/research/20250929091330-128-670951/asia-pukul-balik-amerika-dolar-as-ditendang-won--rupiah-jadi-raja</t>
+          <t>https://www.cnbcindonesia.com/lifestyle/20250929180347-33-671263/bukan-cuma-orang-tua-anak-muda-wajib-waspada-jika-merasa-nyeri-dada</t>
         </is>
       </c>
       <c r="E80" t="inlineStr"/>
@@ -2356,12 +2332,12 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>5 Waktu Terbaik Makan Pisang yang Tak Banyak Orang TahuLifestyle4 jam yang lalu</t>
+          <t>80% Timah RI Diselundupkan, Prabowo Geram dan Siapkan Jurus Ini..News4 jam yang lalu</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2371,7 +2347,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/lifestyle/20250928140454-33-670827/5-waktu-terbaik-makan-pisang-yang-tak-banyak-orang-tahu</t>
+          <t>https://www.cnbcindonesia.com/news/20250930075014-4-671343/80-timah-ri-diselundupkan-prabowo-geram-dan-siapkan-jurus-ini</t>
         </is>
       </c>
       <c r="E81" t="inlineStr"/>
@@ -2379,12 +2355,12 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Harga Saham Bergerak Tak Wajar, BEI Pantau Ketat 5 Emiten IniMarket4 jam yang lalu</t>
+          <t>Omongan Purbaya Bikin Rupiah Balik Perkasa, Ini Ternyata PenjelasannyaNews4 jam yang lalu</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -2394,20 +2370,24 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250929090519-17-670948/harga-saham-bergerak-tak-wajar-bei-pantau-ketat-5-emiten-ini</t>
-        </is>
-      </c>
-      <c r="E82" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/news/20250930084724-4-671365/omongan-purbaya-bikin-rupiah-balik-perkasa-ini-ternyata-penjelasannya</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>purbaya</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Asing Bawa Kabur Rp 42 T, Risiko Gagal Bayar RI Naik DrastisResearch4 jam yang lalu</t>
+          <t>Pasar Tunggu Data Penting, Bursa Asia Dibuka BervariasiMarket4 jam yang lalu</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2417,7 +2397,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/research/20250929081207-128-670925/asing-bawa-kabur-rp-42-t-risiko-gagal-bayar-ri-naik-drastis</t>
+          <t>https://www.cnbcindonesia.com/market/20250930083001-17-671360/pasar-tunggu-data-penting-bursa-asia-dibuka-bervariasi</t>
         </is>
       </c>
       <c r="E83" t="inlineStr"/>
@@ -2425,12 +2405,12 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Daftar Bunga Deposito Rupiah &amp; Dolar BRI, BNI-Mandiri per 29 SeptemberResearch4 jam yang lalu</t>
+          <t>Modus Pedagang Ecommerce, Rokok Ilegal Dijual Jadi Pakaian DalamTech4 jam yang lalu</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2440,7 +2420,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/research/20250929053349-128-670903/daftar-bunga-deposito-rupiah-dolar-bri-bni-mandiri-per-29-september</t>
+          <t>https://www.cnbcindonesia.com/tech/20250930080129-37-671349/modus-pedagang-ecommerce-rokok-ilegal-dijual-jadi-pakaian-dalam</t>
         </is>
       </c>
       <c r="E84" t="inlineStr"/>
@@ -2448,12 +2428,12 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Sepatu Impor Serang Pasar Senen dan Jatinegara, Mereknya Bikin KagetNews4 jam yang lalu</t>
+          <t>Rekor Bersejarah! Harga Emas Antam Logam Mulia Bisa Tembus Rp2,23 JutaResearch5 jam yang lalu</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2463,7 +2443,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250928200659-4-670881/sepatu-impor-serang-pasar-senen-dan-jatinegara-mereknya-bikin-kaget</t>
+          <t>https://www.cnbcindonesia.com/research/20250930083215-128-671363/rekor-bersejarah-harga-emas-antam-logam-mulia-bisa-tembus-rp223-juta</t>
         </is>
       </c>
       <c r="E85" t="inlineStr"/>
@@ -2471,12 +2451,12 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Rekor Lagi! Harga Emas Antam Logam Mulia Hari Ini Hampir Rp 2,2 JutaResearch4 jam yang lalu</t>
+          <t>Antam Ternyata Impor Emas Besar-Besaran, Ini AlasannyaNews5 jam yang lalu</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -2486,7 +2466,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/research/20250929083802-128-670932/rekor-lagi-harga-emas-antam-logam-mulia-hari-ini-hampir-rp-22-juta</t>
+          <t>https://www.cnbcindonesia.com/news/20250930073842-4-671340/antam-ternyata-impor-emas-besar-besaran-ini-alasannya</t>
         </is>
       </c>
       <c r="E86" t="inlineStr"/>
@@ -2494,12 +2474,12 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Bank Syariah Nasional Resmi Dapat Izin Operasi dari OJKMarket4 jam yang lalu</t>
+          <t>10 Saham Ini Ramai Jadi Incaran Asing Kala IHSG HijauMarket5 jam yang lalu</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2509,7 +2489,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250929090720-17-670950/bank-syariah-nasional-resmi-dapat-izin-operasi-dari-ojk</t>
+          <t>https://www.cnbcindonesia.com/market/20250930082703-17-671358/10-saham-ini-ramai-jadi-incaran-asing-kala-ihsg-hijau</t>
         </is>
       </c>
       <c r="E87" t="inlineStr"/>
@@ -2517,12 +2497,12 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>IHSG Dibuka Menguat, Balik Lagi ke Level 8.100Market4 jam yang lalu</t>
+          <t>KPPU: Cara Tiktok Beli Tokopedia Rawan DisalahgunakanTech5 jam yang lalu</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -2532,7 +2512,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250929084220-17-670933/ihsg-dibuka-menguat-balik-lagi-ke-level-8100</t>
+          <t>https://www.cnbcindonesia.com/tech/20250930075711-37-671346/kppu-cara-tiktok-beli-tokopedia-rawan-disalahgunakan</t>
         </is>
       </c>
       <c r="E88" t="inlineStr"/>
@@ -2540,12 +2520,12 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Pemerintah Tetapkan Tarif Listrik Oktober-Desember 2025, Ini DaftarnyaNews4 jam yang lalu</t>
+          <t>Pantas Prabowo Geram! Ada 1.000 Tambang Timah Ilegal di BabelNews5 jam yang lalu</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -2555,7 +2535,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929075531-4-670921/pemerintah-tetapkan-tarif-listrik-oktober-desember-2025-ini-daftarnya</t>
+          <t>https://www.cnbcindonesia.com/news/20250930073414-4-671339/pantas-prabowo-geram-ada-1000-tambang-timah-ilegal-di-babel</t>
         </is>
       </c>
       <c r="E89" t="inlineStr"/>
@@ -2563,12 +2543,12 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Breaking! Rupiah Perkasa, Dolar AS Turun ke Rp16.640Market4 jam yang lalu</t>
+          <t>InternasionalKemlu Respons Baliho Wajah Presiden Prabowo di Tel Aviv IsraelNews5 jam yang lalu</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -2578,7 +2558,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250929082543-17-670927/breaking-rupiah-perkasa-dolar-as-turun-ke-rp16640</t>
+          <t>https://www.cnbcindonesia.com/news/20250930081041-4-671351/kemlu-respons-baliho-wajah-presiden-prabowo-di-tel-aviv-israel</t>
         </is>
       </c>
       <c r="E90" t="inlineStr"/>
@@ -2586,12 +2566,12 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>InternasionalRaja Singa Tiba-Tiba Meledak di Sini, Kasus Naik 460%News4 jam yang lalu</t>
+          <t>Titah Prabowo: TNI-Polri Operasi Besar-Besaran di Babel, Ini AlasannyaNews5 jam yang lalu</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -2601,7 +2581,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250929084616-4-670934/raja-singa-tiba-tiba-meledak-di-sini-kasus-naik-460</t>
+          <t>https://www.cnbcindonesia.com/news/20250930071440-4-671338/titah-prabowo-tni-polri-operasi-besar-besaran-di-babel-ini-alasannya</t>
         </is>
       </c>
       <c r="E91" t="inlineStr"/>

</xml_diff>

<commit_message>
End to end proses ok.
</commit_message>
<xml_diff>
--- a/daftar_berita/cnbc.xlsx
+++ b/daftar_berita/cnbc.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E91"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,12 +463,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>InternasionalTrump Makin Gencar "Invasi" Negeri Sendiri, Kota Ini Siap MelawanNews4 menit yang lalu</t>
+          <t>Resmi! Ini Daftar Tarif Listrik per kWh PLN, Berlaku 1 Oktober 2025News4 menit yang lalu</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -478,7 +478,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930122006-4-671480/trump-makin-gencar-invasi-negeri-sendiri-kota-ini-siap-melawan</t>
+          <t>https://www.cnbcindonesia.com/news/20251001073226-4-671728/resmi-ini-daftar-tarif-listrik-per-kwh-pln-berlaku-1-oktober-2025</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -486,12 +486,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Wamenperin Sebut Produsen Rokok Tak Nikmati Kenaikan Harga, kok bisa?News9 menit yang lalu</t>
+          <t>Pasar Asia Bervariasi Rabu Pagi:Nikkei &amp; Topix Melemah, Kospi MenguatMarket6 menit yang lalu</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -501,7 +501,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930121920-4-671479/wamenperin-sebut-produsen-rokok-tak-nikmati-kenaikan-harga-kok-bisa</t>
+          <t>https://www.cnbcindonesia.com/market/20251001080327-17-671742/pasar-asia-bervariasi-rabu-paginikkei-topix-melemah-kospi-menguat</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -509,12 +509,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Survei Terbaru: Ojol Lebih Suka Potongan 20% untuk Promo &amp; InsentifTech13 menit yang lalu</t>
+          <t>Toko Online Didenda Rp 41 Triliun Karena Menipu PembeliTech9 menit yang lalu</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -524,7 +524,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250930132454-37-671531/survei-terbaru-ojol-lebih-suka-potongan-20-untuk-promo-insentif</t>
+          <t>https://www.cnbcindonesia.com/tech/20251001073104-37-671726/toko-online-didenda-rp-41-triliun-karena-menipu-pembeli</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -532,12 +532,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Purbaya Tegur BUMN: Hati-Hati Salurkan Subsidi!News14 menit yang lalu</t>
+          <t>InternasionalGelap! Pemerintah AS Akan Tutup, Shutdown Mulai Rabu Tengah MalamNews12 menit yang lalu</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -547,24 +547,20 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930114905-4-671464/purbaya-tegur-bumn-hati-hati-salurkan-subsidi</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>purbaya</t>
-        </is>
-      </c>
+          <t>https://www.cnbcindonesia.com/news/20251001083656-4-671751/gelap-pemerintah-as-akan-tutup-shutdown-mulai-rabu-tengah-malam</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Sulap Sampah Jadi Energi, Bos Danantara Beberkan ManfaatnyaMarket18 menit yang lalu</t>
+          <t>Alexander Ramlie Jual 20 Juta Saham Amman (AMMN), Ini TujuannyaMarket19 menit yang lalu</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -574,7 +570,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250930124321-17-671501/sulap-sampah-jadi-energi-bos-danantara-beberkan-manfaatnya</t>
+          <t>https://www.cnbcindonesia.com/market/20251001073311-17-671727/alexander-ramlie-jual-20-juta-saham-amman--ammn--ini-tujuannya</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -582,12 +578,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Bos Danantara Ungkap Investasi Proyek Sampah Jadi Energi Rp2,3 TriliunMarket18 menit yang lalu</t>
+          <t>Cukai Rokok 2026 Tidak Naik, Ekonom: Purbaya Benar, Ini Angin Segar!News23 menit yang lalu</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -597,20 +593,24 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250930132253-17-671529/bos-danantara-ungkap-investasi-proyek-sampah-jadi-energi-rp23-triliun</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/news/20251001072528-4-671724/cukai-rokok-2026-tidak-naik-ekonom-purbaya-benar-ini-angin-segar</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>purbaya</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Dikuasai Asing! 11 Emiten Raksasa RI Ini Dikendalikan Jepang &amp; AmerikaResearch24 menit yang lalu</t>
+          <t>TikTok Purbaya Difollow Ray Dalio, Komentar Begini ke PrabowoTech29 menit yang lalu</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -620,20 +620,24 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/research/20250930093727-128-671385/dikuasai-asing-11-emiten-raksasa-ri-ini-dikendalikan-jepang-amerika</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/tech/20251001080007-37-671740/tiktok-purbaya-difollow-ray-dalio-komentar-begini-ke-prabowo</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>purbaya</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Tanggal Peluncuran iPhone 17 di RI Terungkap, Harga Tembus Rp 42 JutaTech29 menit yang lalu</t>
+          <t>Ilmuwan Ramal Bencana 2030 Dekat RI: Waduk Kering, Air SusahTech29 menit yang lalu</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -643,7 +647,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250930125540-37-671520/tanggal-peluncuran-iphone-17-di-ri-terungkap-harga-tembus-rp-42-juta</t>
+          <t>https://www.cnbcindonesia.com/tech/20251001073535-37-671729/ilmuwan-ramal-bencana-2030-dekat-ri-waduk-kering-air-susah</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -651,12 +655,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Pendapatan Anjlok, Laba Solusi Bangun (SMCB) Naik 63%! Ini PenyebabnyaMarket33 menit yang lalu</t>
+          <t>Ada yang Naik! Ini Daftar Resmi Harga BBM Pertamina, Berlaku 1 OktoberNews34 menit yang lalu</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -666,7 +670,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250930112331-17-671452/pendapatan-anjlok-laba-solusi-bangun--smcb--naik-63-ini-penyebabnya</t>
+          <t>https://www.cnbcindonesia.com/news/20251001071950-4-671722/ada-yang-naik-ini-daftar-resmi-harga-bbm-pertamina-berlaku-1-oktober</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -674,12 +678,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Bukan Keluarga Raja, Ini Orang Terkaya di Dubai Berharta Rp 285 TLifestyle38 menit yang lalu</t>
+          <t>Ekspansi Setipis Kertas: Domestik Selamatkan Manufaktur RI, Ekspor ByeResearch39 menit yang lalu</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -689,7 +693,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/lifestyle/20250930110544-33-671444/bukan-keluarga-raja-ini-orang-terkaya-di-dubai-berharta-rp-285-t</t>
+          <t>https://www.cnbcindonesia.com/research/20251001074859-128-671737/ekspansi-setipis-kertas-domestik-selamatkan-manufaktur-ri-ekspor-bye</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -697,12 +701,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Purbaya Janji Lunasi Tunggakan ke BUMN Rp55 T: Tapi Jangan Rugi Terus!News43 menit yang lalu</t>
+          <t>Internasional7 Update Gaza: Hamas Respons Deal Trump-Netanyahu, Tepi Barat KolapsNews44 menit yang lalu</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -712,24 +716,20 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930125556-4-671517/purbaya-janji-lunasi-tunggakan-ke-bumn-rp55-t-tapi-jangan-rugi-terus</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>purbaya</t>
-        </is>
-      </c>
+          <t>https://www.cnbcindonesia.com/news/20251001072018-4-671721/7-update-gaza-hamas-respons-deal-trump-netanyahu-tepi-barat-kolaps</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>InternasionalIni Reaksi Hamas soal Deal Trump-Netanyahu, Perang Gaza Kelar?News44 menit yang lalu</t>
+          <t>IHSG Koreksi, Asing Diam-Diam Koleksi Saham IniMarket48 menit yang lalu</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -739,7 +739,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930122609-4-671483/ini-reaksi-hamas-soal-deal-trump-netanyahu-perang-gaza-kelar</t>
+          <t>https://www.cnbcindonesia.com/market/20251001063306-17-671710/ihsg-koreksi-asing-diam-diam-koleksi-saham-ini</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -747,12 +747,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Kapan Program Magang Digaji Rp3,3 Juta Dimulai? Begini Kata MenakerNews45 menit yang lalu</t>
+          <t>Orang Terkaya China Tak Lulus SD, Tapi Hartanya Rp1.200 TriliunLifestyle53 menit yang lalu</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -762,7 +762,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930125516-4-671519/kapan-program-magang-digaji-rp33-juta-dimulai-begini-kata-menaker</t>
+          <t>https://www.cnbcindonesia.com/lifestyle/20250930165731-33-671637/orang-terkaya-china-tak-lulus-sd-tapi-hartanya-rp1200-triliun</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
@@ -770,12 +770,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>TASPEN Lakukan Ini Buat Perkuat Transparansi &amp; Efektivitas PengawasanNews49 menit yang lalu</t>
+          <t>1.300 UMKM Antusias Ikuti Kompetisi Perdana 'Shopee Jagoan Naik Kelas'Entrepreneur53 menit yang lalu</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -785,7 +785,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930125507-4-671518/taspen-lakukan-ini-buat-perkuat-transparansi-efektivitas-pengawasan</t>
+          <t>https://www.cnbcindonesia.com/entrepreneur/20250930222730-25-671700/1300-umkm-antusias-ikuti-kompetisi-perdana-shopee-jagoan-naik-kelas</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
@@ -793,12 +793,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>InternasionalRamai Perusahaan Jepang 'Buru' Pekerja WNI, Ini AlasannyaNews54 menit yang lalu</t>
+          <t>Cek! Iuran BPJS Kesehatan Kelas 1,2,3 Berlaku 1 Oktober 2025News58 menit yang lalu</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -808,7 +808,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930122336-4-671481/ramai-perusahaan-jepang-buru-pekerja-wni-ini-alasannya</t>
+          <t>https://www.cnbcindonesia.com/news/20251001071617-4-671720/cek-iuran-bpjs-kesehatan-kelas-123-berlaku-1-oktober-2025</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
@@ -816,12 +816,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Bumi Kedatangan Komet Raksasa Oktober 2025, Ini Penjelasan IlmuwanTech1 jam yang lalu</t>
+          <t>Temuan di China Ubah Sejarah Panjang Asal Usul ManusiaTech1 jam yang lalu</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -831,7 +831,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250930110920-37-671443/bumi-kedatangan-komet-raksasa-oktober-2025-ini-penjelasan-ilmuwan</t>
+          <t>https://www.cnbcindonesia.com/tech/20250930194955-37-671673/temuan-di-china-ubah-sejarah-panjang-asal-usul-manusia</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
@@ -839,12 +839,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Airlangga Hartarto Datangi Langsung Menaker di Kantornya, Ada Apa?News1 jam yang lalu</t>
+          <t>InternasionalShutdown AS di Depan Mata, Trump Tiba-Tiba Beri Warning Ngeri IniNews1 jam yang lalu</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -854,7 +854,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930124008-4-671499/airlangga-hartarto-datangi-langsung-menaker-di-kantornya-ada-apa</t>
+          <t>https://www.cnbcindonesia.com/news/20251001060125-4-671706/shutdown-as-di-depan-mata-trump-tiba-tiba-beri-warning-ngeri-ini</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -862,12 +862,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Erick Thohir Bantah Tuduhan Mengintervensi FIFA atas Sanksi MalaysiaLifestyle1 jam yang lalu</t>
+          <t>Diburu Interpol, Ini Profil Michael Steven Buron yang Dicari OJKMarket1 jam yang lalu</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -877,7 +877,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/lifestyle/20250930111515-33-671459/erick-thohir-bantah-tuduhan-mengintervensi-fifa-atas-sanksi-malaysia</t>
+          <t>https://www.cnbcindonesia.com/market/20250930185507-17-671667/diburu-interpol-ini-profil-michael-steven-buron-yang-dicari-ojk</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
@@ -885,12 +885,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Shutdown Jadi Hantu Abadi Ekonomi AS: Puluhan Presiden Jadi KorbanResearch1 jam yang lalu</t>
+          <t>Wilayah RI Goncang, Langit Amerika Berubah Merah, Bulan MembiruTech1 jam yang lalu</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -900,7 +900,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/research/20250930103308-128-671425/shutdown-jadi-hantu-abadi-ekonomi-as-puluhan-presiden-jadi-korban</t>
+          <t>https://www.cnbcindonesia.com/tech/20251001072559-37-671723/wilayah-ri-goncang-langit-amerika-berubah-merah-bulan-membiru</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
@@ -908,12 +908,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>IHSG Turun 0,33%, Tiga Saham Diburu Saat Emiten Bank Jumbo RontokMarket1 jam yang lalu</t>
+          <t>Ini yang Terjadi di Tubuh Saat Sarapan Telur Rebus vs Nasi Uduk/BuburLifestyle1 jam yang lalu</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -923,7 +923,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250930120706-17-671485/ihsg-turun-033-tiga-saham-diburu-saat-emiten-bank-jumbo-rontok</t>
+          <t>https://www.cnbcindonesia.com/lifestyle/20250930151146-33-671594/ini-yang-terjadi-di-tubuh-saat-sarapan-telur-rebus-vs-nasi-uduk-bubur</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
@@ -931,12 +931,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Sudah Direstrukturisasi, Krakatau Steel Masih Punya Utang Rp 28,37 TMarket1 jam yang lalu</t>
+          <t>BKN Pecat 19 ASN LagiNews1 jam yang lalu</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -946,7 +946,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250930105211-17-671442/sudah-direstrukturisasi-krakatau-steel-masih-punya-utang-rp-2837-t</t>
+          <t>https://www.cnbcindonesia.com/news/20251001065757-4-671718/bkn-pecat-19-asn-lagi</t>
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
@@ -954,12 +954,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Buruh Batalkan Aksi Demo Hari Ini ke DPR, Terungkap AlasannyaNews1 jam yang lalu</t>
+          <t>Pesta 3 Hari Batu Bara Langsung Bubar Gara-Gara Ada Liburan ChinaResearch1 jam yang lalu</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -969,7 +969,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930122350-4-671482/buruh-batalkan-aksi-demo-hari-ini-ke-dpr-terungkap-alasannya</t>
+          <t>https://www.cnbcindonesia.com/research/20251001064831-128-671717/pesta-3-hari-batu-bara-langsung-bubar-gara-gara-ada-liburan-china</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
@@ -977,12 +977,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Purbaya: Sebulan Subsidi &amp; Kompensasi BUMN Tak Dibayar, Dirjen GantiNews1 jam yang lalu</t>
+          <t>Asing Net Sell Jumbo Rp 1,7 T Sehari, BBCA Paling Banyak DijualMarket1 jam yang lalu</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -992,24 +992,20 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930120753-4-671469/purbaya-sebulan-subsidi-kompensasi-bumn-tak-dibayar-dirjen-ganti</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>purbaya</t>
-        </is>
-      </c>
+          <t>https://www.cnbcindonesia.com/market/20251001062651-17-671709/asing-net-sell-jumbo-rp-17-t-sehari-bbca-paling-banyak-dijual</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Bos Badan Pangan Ingatkan Beras Busuk Tak Boleh Diedarkan, Stok Aman?News1 jam yang lalu</t>
+          <t>Era Mobil Bensin Segera Berakhir Berkat Temuan Baru Peneliti KoreaTech1 jam yang lalu</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1019,7 +1015,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930111012-4-671445/bos-badan-pangan-ingatkan-beras-busuk-tak-boleh-diedarkan-stok-aman</t>
+          <t>https://www.cnbcindonesia.com/tech/20250930200035-37-671675/era-mobil-bensin-segera-berakhir-berkat-temuan-baru-peneliti-korea</t>
         </is>
       </c>
       <c r="E25" t="inlineStr"/>
@@ -1027,12 +1023,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Ekosistem Baterai UV Ubah Paradigma Ekonomi IndonesiaOpini1 jam yang lalu</t>
+          <t>InternasionalLagi Perang Saudara, Tetangga RI Ini Kebut Bangun Nuklir Dibantu RusiaNews1 jam yang lalu</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1042,7 +1038,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/opini/20250930103621-14-671429/ekosistem-baterai-uv-ubah-paradigma-ekonomi-indonesia</t>
+          <t>https://www.cnbcindonesia.com/news/20251001033810-4-671703/lagi-perang-saudara-tetangga-ri-ini-kebut-bangun-nuklir-dibantu-rusia</t>
         </is>
       </c>
       <c r="E26" t="inlineStr"/>
@@ -1050,12 +1046,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Soal Subsidi 2024, Purbaya: Jika Ada yang Belum Dibayar Hadap Saya!News1 jam yang lalu</t>
+          <t>Purbaya Cek Langsung Proyek BUMN, Tak Jalan Bakal Dapat GanjaranNews1 jam yang lalu</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1065,7 +1061,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930120705-4-671468/soal-subsidi-2024-purbaya-jika-ada-yang-belum-dibayar-hadap-saya</t>
+          <t>https://www.cnbcindonesia.com/news/20250930153307-4-671603/purbaya-cek-langsung-proyek-bumn-tak-jalan-bakal-dapat-ganjaran</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1077,12 +1073,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>NASA Temukan Tanda Kehidupan Paling Jelas di Mars, Cek FaktanyaTech1 jam yang lalu</t>
+          <t>Mendadak Komisi III DPR Bahas Kasus Maybank, Ini KronologinyaMarket2 jam yang lalu</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1092,7 +1088,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250930104626-37-671437/nasa-temukan-tanda-kehidupan-paling-jelas-di-mars-cek-faktanya</t>
+          <t>https://www.cnbcindonesia.com/market/20250930174905-17-671647/mendadak-komisi-iii-dpr-bahas-kasus-maybank-ini-kronologinya</t>
         </is>
       </c>
       <c r="E28" t="inlineStr"/>
@@ -1100,12 +1096,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Terungkap! Bandung Bakal Punya KRL, Rutenya IniNews1 jam yang lalu</t>
+          <t>Kisah Kirim Emoji Jempol Kena Denda Nyaris Rp 1 MiliarTech2 jam yang lalu</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1115,7 +1111,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930115522-4-671466/terungkap-bandung-bakal-punya-krl-rutenya-ini</t>
+          <t>https://www.cnbcindonesia.com/tech/20250930200546-37-671680/kisah-kirim-emoji-jempol-kena-denda-nyaris-rp-1-miliar</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
@@ -1123,12 +1119,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Bos Danantara Blak-Blakan Soal Merger Asuransi BUMN, IFG Jadi HoldingMarket1 jam yang lalu</t>
+          <t>Harga Emas Ngebut Tanpa Rem: Setiap Hari Pecah Rekor, Kapan Berhenti?Research2 jam yang lalu</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1138,7 +1134,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250930115445-17-671467/bos-danantara-blak-blakan-soal-merger-asuransi-bumn-ifg-jadi-holding</t>
+          <t>https://www.cnbcindonesia.com/research/20251001054522-128-671705/harga-emas-ngebut-tanpa-rem-setiap-hari-pecah-rekor-kapan-berhenti</t>
         </is>
       </c>
       <c r="E30" t="inlineStr"/>
@@ -1146,12 +1142,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>InternasionalPerang Dagang Lagi! Trump Umumkan Tarif Baru, 25%-50% Mulai 14 OktoberNews1 jam yang lalu</t>
+          <t>NewsletterBadai Sentimen Mengintai RI: Inflasi, Ekonomi China &amp; Shutdown AmerikaResearch2 jam yang lalu</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1161,7 +1157,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930115046-4-671465/perang-dagang-lagi-trump-umumkan-tarif-baru-25-50-mulai-14-oktober</t>
+          <t>https://www.cnbcindonesia.com/research/20250930214623-128-671698/badai-sentimen-mengintai-ri-inflasi-ekonomi-china-shutdown-amerika</t>
         </is>
       </c>
       <c r="E31" t="inlineStr"/>
@@ -1169,12 +1165,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Purbaya Ungkap Harga Sebenarnya Pertalite, Solar Sampai LPGNews1 jam yang lalu</t>
+          <t>InternasionalKala Trump Puji Prabowo Secara Langsung Depan Netanyahu, Katakan IniNews2 jam yang lalu</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1184,24 +1180,20 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930112226-4-671449/purbaya-ungkap-harga-sebenarnya-pertalite-solar-sampai-lpg</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>purbaya</t>
-        </is>
-      </c>
+          <t>https://www.cnbcindonesia.com/news/20251001032306-4-671702/kala-trump-puji-prabowo-secara-langsung-depan-netanyahu-katakan-ini</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>InternasionalPMI Manufaktur China Kontraksi, Enam Kali Berturut-turutNews1 jam yang lalu</t>
+          <t>Memperkuat Ekosistem Zakat, Strategi Mewujudkan Kemakmuran BangsaOpini3 jam yang lalu</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1211,7 +1203,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930113331-4-671455/pmi-manufaktur-china-kontraksi-enam-kali-berturut-turut</t>
+          <t>https://www.cnbcindonesia.com/opini/20251001053444-14-671704/memperkuat-ekosistem-zakat-strategi-mewujudkan-kemakmuran-bangsa</t>
         </is>
       </c>
       <c r="E33" t="inlineStr"/>
@@ -1219,12 +1211,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>BUMN Jangan Khawatir, Purbaya Siap Bayar Subsidi Oktober 2025News1 jam yang lalu</t>
+          <t>Target Pertumbuhan Ekonomi 8% dan Penurunan Pengangguran SarjanaOpini3 jam yang lalu</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1234,24 +1226,20 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930114552-4-671458/bumn-jangan-khawatir-purbaya-siap-bayar-subsidi-oktober-2025</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>purbaya</t>
-        </is>
-      </c>
+          <t>https://www.cnbcindonesia.com/opini/20250930134854-14-671540/target-pertumbuhan-ekonomi-8-dan-penurunan-pengangguran-sarjana</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Rupiah Perkasa Lawan Dolar, Ekonom Ungkap Penyebab UtamanyaNews1 jam yang lalu</t>
+          <t>Gempa Bumi M 6,5 Guncang Sumenep Madura, Kedalaman 11 KmNews3 jam yang lalu</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1261,7 +1249,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930114126-4-671457/rupiah-perkasa-lawan-dolar-ekonom-ungkap-penyebab-utamanya</t>
+          <t>https://www.cnbcindonesia.com/news/20251001025323-4-671701/gempa-bumi-m-65-guncang-sumenep-madura-kedalaman-11-km</t>
         </is>
       </c>
       <c r="E35" t="inlineStr"/>
@@ -1269,12 +1257,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>6 Alasan Kenapa Harga Emas Bisa Meledak ke LangitResearch1 jam yang lalu</t>
+          <t>InternasionalDeal Perdamaian Gaza ala Trump-Netanyahu, 5 Hal Ini Masih Tanda TanyaNews10 jam yang lalu</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1284,7 +1272,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/research/20250930104459-128-671436/6-alasan-kenapa-harga-emas-bisa-meledak-ke-langit</t>
+          <t>https://www.cnbcindonesia.com/news/20250930133153-4-671533/deal-perdamaian-gaza-ala-trump-netanyahu-5-hal-ini-masih-tanda-tanya</t>
         </is>
       </c>
       <c r="E36" t="inlineStr"/>
@@ -1292,12 +1280,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Green Era Energy Kembali Jual Saham BREN, Kali Ini Raup Rp698 MiliarMarket2 jam yang lalu</t>
+          <t>Resmi! Pertamina Tetapkan Harga BBM Non Subsidi per 1 OktoberNews11 jam yang lalu</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1307,7 +1295,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250930091033-17-671374/green-era-energy-kembali-jual-saham-bren-kali-ini-raup-rp698-miliar</t>
+          <t>https://www.cnbcindonesia.com/news/20250930215128-4-671699/resmi-pertamina-tetapkan-harga-bbm-non-subsidi-per-1-oktober</t>
         </is>
       </c>
       <c r="E37" t="inlineStr"/>
@@ -1315,12 +1303,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Pengusaha Baja Teriak, RI Lemah Lawan Serbuan Barang Impor &amp; DumpingNews2 jam yang lalu</t>
+          <t>Kolaborasi Shopee dan Vidio, Belanja Langsung dari Tayangan Favorit!Tech11 jam yang lalu</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1330,7 +1318,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930103725-4-671431/pengusaha-baja-teriak-ri-lemah-lawan-serbuan-barang-impor-dumping</t>
+          <t>https://www.cnbcindonesia.com/tech/20250930213906-37-671697/kolaborasi-shopee-dan-vidio-belanja-langsung-dari-tayangan-favorit</t>
         </is>
       </c>
       <c r="E38" t="inlineStr"/>
@@ -1338,12 +1326,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Pasien Alzheimer Termuda Dunia Baru 19 Tahun, Ahli Saraf BingungLifestyle2 jam yang lalu</t>
+          <t>ICW: Penanganan Korupsi Turun Drastis, 364 Kasus Tak Disidik di 2024News11 jam yang lalu</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1353,7 +1341,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/lifestyle/20250930104202-33-671434/pasien-alzheimer-termuda-dunia-baru-19-tahun-ahli-saraf-bingung</t>
+          <t>https://www.cnbcindonesia.com/news/20250930200052-4-671676/icw-penanganan-korupsi-turun-drastis-364-kasus-tak-disidik-di-2024</t>
         </is>
       </c>
       <c r="E39" t="inlineStr"/>
@@ -1361,12 +1349,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Ada Transaksi Jumbo di MMLP, Astra Resmi Jadi Pengendali Baru?Market2 jam yang lalu</t>
+          <t>InternasionalEropa Pecah! Negara Ini Sebut Zelensky Gila-Ragukan Kedaulatan UkrainaNews11 jam yang lalu</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1376,7 +1364,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250930111133-17-671453/ada-transaksi-jumbo-di-mmlp-astra-resmi-jadi-pengendali-baru</t>
+          <t>https://www.cnbcindonesia.com/news/20250930074721-4-671341/eropa-pecah-negara-ini-sebut-zelensky-gila-ragukan-kedaulatan-ukraina</t>
         </is>
       </c>
       <c r="E40" t="inlineStr"/>
@@ -1384,12 +1372,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Pesawat Diserang Maling, Nasib Penumpang MemprihatinkanTech2 jam yang lalu</t>
+          <t>Inalum Naikkan Produksi Aluminium 4 Kali Lipat di 2029, Begini CaranyaNews11 jam yang lalu</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1399,7 +1387,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250930103605-37-671428/pesawat-diserang-maling-nasib-penumpang-memprihatinkan</t>
+          <t>https://www.cnbcindonesia.com/news/20250930144136-4-671567/inalum-naikkan-produksi-aluminium-4-kali-lipat-di-2029-begini-caranya</t>
         </is>
       </c>
       <c r="E41" t="inlineStr"/>
@@ -1407,12 +1395,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>BULL Private Placement Rp254 Miliar, Investor Hong Kong Jadi PemborongMarket2 jam yang lalu</t>
+          <t>InternasionalMengenal Rudal Tomahawk AS, Idaman Ukraina-Mimpi Buruk RusiaNews11 jam yang lalu</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1422,7 +1410,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250930100439-17-671417/bull-private-placement-rp254-miliar-investor-hong-kong-jadi-pemborong</t>
+          <t>https://www.cnbcindonesia.com/news/20250930183921-4-671664/mengenal-rudal-tomahawk-as-idaman-ukraina-mimpi-buruk-rusia</t>
         </is>
       </c>
       <c r="E42" t="inlineStr"/>
@@ -1430,12 +1418,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Purbaya Lapor ke DPR, Subsidi BBM Cs 2025 Tembus Rp479 TNews2 jam yang lalu</t>
+          <t>Ulah China Bikin AS Kebakaran Jenggot, Krisis Besar Mengancam DuniaTech11 jam yang lalu</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1445,24 +1433,20 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930111917-4-671448/purbaya-lapor-ke-dpr-subsidi-bbm-cs-2025-tembus-rp479-t</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>purbaya</t>
-        </is>
-      </c>
+          <t>https://www.cnbcindonesia.com/tech/20250930153023-37-671597/ulah-china-bikin-as-kebakaran-jenggot-krisis-besar-mengancam-dunia</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Purbaya Pede Investor Asing Bakal Serbu RI: Mereka Bakal Menikmati!Market2 jam yang lalu</t>
+          <t>InternasionalDiajak Perang &amp; Terancam Invasi AS, Negara Ini Siapkan Status DaruratNews12 jam yang lalu</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1472,24 +1456,20 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250930090917-17-671370/purbaya-pede-investor-asing-bakal-serbu-ri-mereka-bakal-menikmati</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>purbaya</t>
-        </is>
-      </c>
+          <t>https://www.cnbcindonesia.com/news/20250930180602-4-671653/diajak-perang-terancam-invasi-as-negara-ini-siapkan-status-darurat</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Bukan Surabaya, Kereta Cepat RI Ternyata Dirancang Tembus Sampai SiniNews2 jam yang lalu</t>
+          <t>Bos BKPM Ramal Perdagangan RI dan Eropa Bisa Tembus US$60 Juta di 2030News12 jam yang lalu</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1499,7 +1479,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930111016-4-671446/bukan-surabaya-kereta-cepat-ri-ternyata-dirancang-tembus-sampai-sini</t>
+          <t>https://www.cnbcindonesia.com/news/20250930171819-4-671643/bos-bkpm-ramal-perdagangan-ri-dan-eropa-bisa-tembus-us-60-juta-di-2030</t>
         </is>
       </c>
       <c r="E45" t="inlineStr"/>
@@ -1507,12 +1487,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Cukai Rokok Tak Naik, Wamenperin: Perusahaan Cuma Menikmati 20%News2 jam yang lalu</t>
+          <t>Inalum Setor Dividen Rp 2 Triliun ke MIND ID di 2024News12 jam yang lalu</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1522,24 +1502,20 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930102534-4-671423/cukai-rokok-tak-naik-wamenperin-perusahaan-cuma-menikmati-20</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>cukai</t>
-        </is>
-      </c>
+          <t>https://www.cnbcindonesia.com/news/20250930145926-4-671572/inalum-setor-dividen-rp-2-triliun-ke-mind-id-di-2024</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Sillicon Valley Connection Jual 10 Juta Saham WGSH, Nilainya TerungkapMarket2 jam yang lalu</t>
+          <t>Cerita Ray Dalio Puji Langkah Menkeu PurbayaNews12 jam yang lalu</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1549,7 +1525,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250930101106-17-671419/sillicon-valley-connection-jual-10-juta-saham-wgsh-nilainya-terungkap</t>
+          <t>https://www.cnbcindonesia.com/news/20250930200652-4-671682/cerita-ray-dalio-puji-langkah-menkeu-purbaya</t>
         </is>
       </c>
       <c r="E47" t="inlineStr"/>
@@ -1557,12 +1533,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Bos Antam Beberkan Susahnya Dapat Pasokan Emas dari Tambang RINews2 jam yang lalu</t>
+          <t>Matahari Picu Serangan Jantung, Cek Sederet PenelitiannyaTech12 jam yang lalu</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1572,7 +1548,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930103114-4-671430/bos-antam-beberkan-susahnya-dapat-pasokan-emas-dari-tambang-ri</t>
+          <t>https://www.cnbcindonesia.com/tech/20250930133145-37-671560/matahari-picu-serangan-jantung-cek-sederet-penelitiannya</t>
         </is>
       </c>
       <c r="E48" t="inlineStr"/>
@@ -1580,12 +1556,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Purbaya Bertandang ke DPR, Lapor Realisasi Subsidi &amp; KompensasiNews2 jam yang lalu</t>
+          <t>Purbaya Ingatkan BUMN Soal Subsidi: Awas Kalau Ada yang Nyeleweng!News12 jam yang lalu</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1595,7 +1571,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930105425-4-671441/purbaya-bertandang-ke-dpr-lapor-realisasi-subsidi-kompensasi</t>
+          <t>https://www.cnbcindonesia.com/news/20250930170533-4-671639/purbaya-ingatkan-bumn-soal-subsidi-awas-kalau-ada-yang-nyeleweng</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -1607,12 +1583,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Internet Diblokir Total, Penerbangan Batal-Negara Gelap GulitaTech2 jam yang lalu</t>
+          <t>HP Baru Xiaomi Pakai Kamera Leica, Harga Tak Sampai Rp 10 JutaTech12 jam yang lalu</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1622,7 +1598,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250930101257-37-671418/internet-diblokir-total-penerbangan-batal-negara-gelap-gulita</t>
+          <t>https://www.cnbcindonesia.com/tech/20250930194537-37-671671/hp-baru-xiaomi-pakai-kamera-leica-harga-tak-sampai-rp-10-juta</t>
         </is>
       </c>
       <c r="E50" t="inlineStr"/>
@@ -1630,12 +1606,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Bos Danantara Ungkap RI Darurat Sampah, Jumlahnya 16.500 Lapangan BolaMarket2 jam yang lalu</t>
+          <t>Ekonomi Akhir 2025 Bisa Tumbuh 5,5%, Purbaya Bocorkan PendorongnyaNews13 jam yang lalu</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1645,20 +1621,24 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250930104814-17-671440/bos-danantara-ungkap-ri-darurat-sampah-jumlahnya-16500-lapangan-bola</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/news/20250930163611-4-671629/ekonomi-akhir-2025-bisa-tumbuh-55-purbaya-bocorkan-pendorongnya</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>purbaya</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Komisi XI DPR Buka-bukaan Soal Proses Pembahasan RUU P2SK, Simak!News2 jam yang lalu</t>
+          <t>NASA Mau Pasang Wi-Fi di Bulan, Biayanya Rp 2,5 MiliarTech13 jam yang lalu</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1668,7 +1648,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930101809-4-671420/komisi-xi-dpr-buka-bukaan-soal-proses-pembahasan-ruu-p2sk-simak</t>
+          <t>https://www.cnbcindonesia.com/tech/20250930154435-37-671606/nasa-mau-pasang-wi-fi-di-bulan-biayanya-rp-25-miliar</t>
         </is>
       </c>
       <c r="E52" t="inlineStr"/>
@@ -1676,12 +1656,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>MIND ID Perkuat Kinerja Lewat Inovasi Hilirisasi MineralNews3 jam yang lalu</t>
+          <t>Aplikasi Pengganti TikTok Buatan AS Segera Rilis, Jauh Lebih CanggihTech13 jam yang lalu</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1691,7 +1671,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930104358-4-671435/mind-id-perkuat-kinerja-lewat-inovasi-hilirisasi-mineral</t>
+          <t>https://www.cnbcindonesia.com/tech/20250930160744-37-671620/aplikasi-pengganti-tiktok-buatan-as-segera-rilis-jauh-lebih-canggih</t>
         </is>
       </c>
       <c r="E53" t="inlineStr"/>
@@ -1699,12 +1679,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Pasar Kelebihan Pasokan, Harga Minyak Dunia AnjlokMarket3 jam yang lalu</t>
+          <t>Usai Diterima Prabowo di Istana, Begini Kata Marc MarquezNews13 jam yang lalu</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1714,7 +1694,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250930094657-17-671393/pasar-kelebihan-pasokan-harga-minyak-dunia-anjlok</t>
+          <t>https://www.cnbcindonesia.com/news/20250930182411-4-671663/usai-diterima-prabowo-di-istana-begini-kata-marc-marquez</t>
         </is>
       </c>
       <c r="E54" t="inlineStr"/>
@@ -1722,12 +1702,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Duel Sengit: RI vs Malaysia Saling Tikung Akuisisi Emiten RaksasaResearch3 jam yang lalu</t>
+          <t>Marc Marquez Temui Prabowo di Istana Jelang MotoGP MandalikaLifestyle13 jam yang lalu</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1737,7 +1717,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/research/20250930093928-128-671387/duel-sengit-ri-vs-malaysia-saling-tikung-akuisisi-emiten-raksasa</t>
+          <t>https://www.cnbcindonesia.com/lifestyle/20250930192724-33-671670/marc-marquez-temui-prabowo-di-istana-jelang-motogp-mandalika</t>
         </is>
       </c>
       <c r="E55" t="inlineStr"/>
@@ -1745,12 +1725,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>3 Emiten Teknologi Mau Rights Issue, Galang Dana Lebih dari Rp 9 TMarket3 jam yang lalu</t>
+          <t>Alasan Ilmiah Kenapa Sering Stress Bikin Wajah Terlihat Lebih TuaLifestyle13 jam yang lalu</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1760,7 +1740,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/market/20250930093044-17-671386/3-emiten-teknologi-mau-rights-issue-galang-dana-lebih-dari-rp-9-t</t>
+          <t>https://www.cnbcindonesia.com/lifestyle/20250930161917-33-671635/alasan-ilmiah-kenapa-sering-stress-bikin-wajah-terlihat-lebih-tua</t>
         </is>
       </c>
       <c r="E56" t="inlineStr"/>
@@ -1768,12 +1748,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>InternasionalNetanyahu Tiba-Tiba Minta Maaf ke Pemimpin Arab, Janji Tak Ulangi LagiNews3 jam yang lalu</t>
+          <t>Xiaomi 15T Series Rilis di RI Harga Mulai Rp6 Juta, Ini SpesifikasinyaTech13 jam yang lalu</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1783,7 +1763,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930102040-4-671422/netanyahu-tiba-tiba-minta-maaf-ke-pemimpin-arab-janji-tak-ulangi-lagi</t>
+          <t>https://www.cnbcindonesia.com/tech/20250930191243-37-671669/xiaomi-15t-series-rilis-di-ri-harga-mulai-rp6-juta-ini-spesifikasinya</t>
         </is>
       </c>
       <c r="E57" t="inlineStr"/>
@@ -1791,12 +1771,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Janji Prabowo Bisa Selamatkan Uang Negara Rp 67 Triliun, Ini SumbernyaNews3 jam yang lalu</t>
+          <t>Purbaya Tak Naikkan Cukai Rokok: Masyarakat Perlu PenghidupanNews13 jam yang lalu</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1806,20 +1786,24 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930102537-4-671424/janji-prabowo-bisa-selamatkan-uang-negara-rp-67-triliun-ini-sumbernya</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr"/>
+          <t>https://www.cnbcindonesia.com/news/20250930181235-4-671656/purbaya-tak-naikkan-cukai-rokok-masyarakat-perlu-penghidupan</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>purbaya</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Ikut Kata Prabowo, Bulog Mau Bangun 100 Gudang-Ini LokasinyaNews3 jam yang lalu</t>
+          <t>InternasionalPanas Perang Saudara! Bom Guncang Markas Paramiliter-10 Orang TewasNews13 jam yang lalu</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1829,7 +1813,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930101835-4-671421/ikut-kata-prabowo-bulog-mau-bangun-100-gudang-ini-lokasinya</t>
+          <t>https://www.cnbcindonesia.com/news/20250930174023-4-671645/panas-perang-saudara-bom-guncang-markas-paramiliter-10-orang-tewas</t>
         </is>
       </c>
       <c r="E59" t="inlineStr"/>
@@ -1837,12 +1821,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Purbaya Ramal Ekonomi Kuartal IV-2025 di Atas 5,5%News3 jam yang lalu</t>
+          <t>Malaysia Resmi Turunkan Harga BBM RON 95, Segini Bedanya dengan RINews13 jam yang lalu</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1852,24 +1836,20 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/news/20250930094808-4-671395/purbaya-ramal-ekonomi-kuartal-iv-2025-di-atas-55</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>purbaya</t>
-        </is>
-      </c>
+          <t>https://www.cnbcindonesia.com/news/20250930180306-16-671652/malaysia-resmi-turunkan-harga-bbm-ron-95-segini-bedanya-dengan-ri</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Arab Beli Pencipta Game FIFA Rp 917 Triliun, Menantu Trump PatunganTech3 jam yang lalu</t>
+          <t>6 Fitur WhatsApp Terbaru 2025, Tak Banyak Orang TahuTech13 jam yang lalu</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1879,712 +1859,10 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>https://www.cnbcindonesia.com/tech/20250930082722-37-671359/arab-beli-pencipta-game-fifa-rp-917-triliun-menantu-trump-patungan</t>
+          <t>https://www.cnbcindonesia.com/tech/20250930152532-37-671592/6-fitur-whatsapp-terbaru-2025-tak-banyak-orang-tahu</t>
         </is>
       </c>
       <c r="E61" t="inlineStr"/>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>Selama Ini Terbuang Sia-Sia, Limbah Timah Bernilai Fantastis!News3 jam yang lalu</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>Tidak Diketahui</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>https://www.cnbcindonesia.com/news/20250930092943-4-671379/selama-ini-terbuang-sia-sia-limbah-timah-bernilai-fantastis</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr"/>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>Harga Saham Naik Ratusan Persen, BEI Gembok 7 Emiten SekaligusMarket3 jam yang lalu</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>Tidak Diketahui</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>https://www.cnbcindonesia.com/market/20250930090711-17-671372/harga-saham-naik-ratusan-persen-bei-gembok-7-emiten-sekaligus</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr"/>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>6 Profesi Paling Tidak Dipercaya Masyarakat Menurut SurveiLifestyle3 jam yang lalu</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>Tidak Diketahui</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>https://www.cnbcindonesia.com/lifestyle/20250930085746-33-671367/6-profesi-paling-tidak-dipercaya-masyarakat-menurut-survei</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr"/>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>InternasionalTetangga RI 'Macan Asia' Terancam Resesi, Bakal Kena di 2040News3 jam yang lalu</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>Tidak Diketahui</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>https://www.cnbcindonesia.com/news/20250930095211-4-671402/tetangga-ri-macan-asia-terancam-resesi-bakal-kena-di-2040</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr"/>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>Danantara Bahas Proyek Sampah Jadi Energi, Ray Dalio Terlihat HadirMarket3 jam yang lalu</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>Tidak Diketahui</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>https://www.cnbcindonesia.com/market/20250930094539-17-671392/danantara-bahas-proyek-sampah-jadi-energi-ray-dalio-terlihat-hadir</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr"/>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>Pengumuman! Kantor Purbaya Lelang Alat Pijat, Balon Sampai SapiNews3 jam yang lalu</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>Tidak Diketahui</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>https://www.cnbcindonesia.com/news/20250930092520-4-671377/pengumuman-kantor-purbaya-lelang-alat-pijat-balon-sampai-sapi</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>purbaya</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>Tiba-Tiba Asia Jadi Lautan Merah, Rupiah - Yen Terbakar Dolar ASResearch4 jam yang lalu</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>Tidak Diketahui</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>https://www.cnbcindonesia.com/research/20250930093808-128-671389/tiba-tiba-asia-jadi-lautan-merah-rupiah--yen-terbakar-dolar-as</t>
-        </is>
-      </c>
-      <c r="E68" t="inlineStr"/>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>Pemilik Cadangan Top 5 Dunia Tapi RI Masih Impor Emas Besar-besaran!News4 jam yang lalu</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>Tidak Diketahui</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>https://www.cnbcindonesia.com/news/20250930091732-4-671375/pemilik-cadangan-top-5-dunia-tapi-ri-masih-impor-emas-besar-besaran</t>
-        </is>
-      </c>
-      <c r="E69" t="inlineStr"/>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>Taspen Serahkan Uang Pensiun ke Sri Mulyani, Netizen PenasaranTech4 jam yang lalu</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>Tidak Diketahui</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>https://www.cnbcindonesia.com/tech/20250930091955-37-671376/taspen-serahkan-uang-pensiun-ke-sri-mulyani-netizen-penasaran</t>
-        </is>
-      </c>
-      <c r="E70" t="inlineStr"/>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>Prabowo Sebut BUMN Rugi Bagi Bonus Brengsek, Mau Kirim KPK &amp; KejaksaanMarket4 jam yang lalu</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>Tidak Diketahui</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>https://www.cnbcindonesia.com/market/20250930083834-17-671364/prabowo-sebut-bumn-rugi-bagi-bonus-brengsek-mau-kirim-kpk-kejaksaan</t>
-        </is>
-      </c>
-      <c r="E71" t="inlineStr"/>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>Purbaya Tunda Pungutan PPh Pedagang Online, Ini Kata EcommerceTech4 jam yang lalu</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>Tidak Diketahui</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>https://www.cnbcindonesia.com/tech/20250930091052-37-671371/purbaya-tunda-pungutan-pph-pedagang-online-ini-kata-ecommerce</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>purbaya</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>Harga Saham Bergerak Tak Wajar, BEI Pantau Ketat 3 Emiten IniMarket4 jam yang lalu</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>Tidak Diketahui</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>https://www.cnbcindonesia.com/market/20250930083358-17-671361/harga-saham-bergerak-tak-wajar-bei-pantau-ketat-3-emiten-ini</t>
-        </is>
-      </c>
-      <c r="E73" t="inlineStr"/>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>Peta Timah ASEAN: Laba Jeblok, TINS Tetap Lebih Gahar vs MSC MalaysiaResearch4 jam yang lalu</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>Tidak Diketahui</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>https://www.cnbcindonesia.com/research/20250929125217-128-671078/peta-timah-asean-laba-jeblok-tins-tetap-lebih-gahar-vs-msc-malaysia</t>
-        </is>
-      </c>
-      <c r="E74" t="inlineStr"/>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>Danantara Adakan Rapat, Bahas Proyek Sampah Jadi EnergiMarket4 jam yang lalu</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>Tidak Diketahui</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>https://www.cnbcindonesia.com/market/20250930091639-17-671373/danantara-adakan-rapat-bahas-proyek-sampah-jadi-energi</t>
-        </is>
-      </c>
-      <c r="E75" t="inlineStr"/>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>Skandal Naturalisasi Timnas Malaysia, 7 Pemain Kena Sanksi FIFALifestyle4 jam yang lalu</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>Tidak Diketahui</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>https://www.cnbcindonesia.com/lifestyle/20250930085305-33-671366/skandal-naturalisasi-timnas-malaysia-7-pemain-kena-sanksi-fifa</t>
-        </is>
-      </c>
-      <c r="E76" t="inlineStr"/>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>InternasionalIsi Proposal Perdamaian Gaza Trump-Netanyahu, Arab &amp; RI Disebut SetujuNews4 jam yang lalu</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>Tidak Diketahui</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>https://www.cnbcindonesia.com/news/20250930090324-4-671369/isi-proposal-perdamaian-gaza-trump-netanyahu-arab-ri-disebut-setuju</t>
-        </is>
-      </c>
-      <c r="E77" t="inlineStr"/>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>Rupiah Kembali Menguat, Dolar AS Dibuka Turun ke Rp16.650Market4 jam yang lalu</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>Tidak Diketahui</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>https://www.cnbcindonesia.com/market/20250930083512-17-671362/rupiah-kembali-menguat-dolar-as-dibuka-turun-ke-rp16650</t>
-        </is>
-      </c>
-      <c r="E78" t="inlineStr"/>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>Lanjutkan Reli, IHSG Dibuka Menguat Tipis 0,18% ke 8.137Market4 jam yang lalu</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>Tidak Diketahui</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>https://www.cnbcindonesia.com/market/20250930085009-17-671368/lanjutkan-reli-ihsg-dibuka-menguat-tipis-018-ke-8137</t>
-        </is>
-      </c>
-      <c r="E79" t="inlineStr"/>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>Bukan Cuma Orang Tua, Anak Muda Wajib Waspada Jika Merasa Nyeri DadaLifestyle4 jam yang lalu</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>Tidak Diketahui</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>https://www.cnbcindonesia.com/lifestyle/20250929180347-33-671263/bukan-cuma-orang-tua-anak-muda-wajib-waspada-jika-merasa-nyeri-dada</t>
-        </is>
-      </c>
-      <c r="E80" t="inlineStr"/>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>80% Timah RI Diselundupkan, Prabowo Geram dan Siapkan Jurus Ini..News4 jam yang lalu</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>Tidak Diketahui</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>https://www.cnbcindonesia.com/news/20250930075014-4-671343/80-timah-ri-diselundupkan-prabowo-geram-dan-siapkan-jurus-ini</t>
-        </is>
-      </c>
-      <c r="E81" t="inlineStr"/>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>Omongan Purbaya Bikin Rupiah Balik Perkasa, Ini Ternyata PenjelasannyaNews4 jam yang lalu</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>Tidak Diketahui</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>https://www.cnbcindonesia.com/news/20250930084724-4-671365/omongan-purbaya-bikin-rupiah-balik-perkasa-ini-ternyata-penjelasannya</t>
-        </is>
-      </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>purbaya</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>Pasar Tunggu Data Penting, Bursa Asia Dibuka BervariasiMarket4 jam yang lalu</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>Tidak Diketahui</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>https://www.cnbcindonesia.com/market/20250930083001-17-671360/pasar-tunggu-data-penting-bursa-asia-dibuka-bervariasi</t>
-        </is>
-      </c>
-      <c r="E83" t="inlineStr"/>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>Modus Pedagang Ecommerce, Rokok Ilegal Dijual Jadi Pakaian DalamTech4 jam yang lalu</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>Tidak Diketahui</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>https://www.cnbcindonesia.com/tech/20250930080129-37-671349/modus-pedagang-ecommerce-rokok-ilegal-dijual-jadi-pakaian-dalam</t>
-        </is>
-      </c>
-      <c r="E84" t="inlineStr"/>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>Rekor Bersejarah! Harga Emas Antam Logam Mulia Bisa Tembus Rp2,23 JutaResearch5 jam yang lalu</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>Tidak Diketahui</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>https://www.cnbcindonesia.com/research/20250930083215-128-671363/rekor-bersejarah-harga-emas-antam-logam-mulia-bisa-tembus-rp223-juta</t>
-        </is>
-      </c>
-      <c r="E85" t="inlineStr"/>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>Antam Ternyata Impor Emas Besar-Besaran, Ini AlasannyaNews5 jam yang lalu</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>Tidak Diketahui</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>https://www.cnbcindonesia.com/news/20250930073842-4-671340/antam-ternyata-impor-emas-besar-besaran-ini-alasannya</t>
-        </is>
-      </c>
-      <c r="E86" t="inlineStr"/>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>10 Saham Ini Ramai Jadi Incaran Asing Kala IHSG HijauMarket5 jam yang lalu</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>Tidak Diketahui</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>https://www.cnbcindonesia.com/market/20250930082703-17-671358/10-saham-ini-ramai-jadi-incaran-asing-kala-ihsg-hijau</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr"/>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>KPPU: Cara Tiktok Beli Tokopedia Rawan DisalahgunakanTech5 jam yang lalu</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>Tidak Diketahui</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>https://www.cnbcindonesia.com/tech/20250930075711-37-671346/kppu-cara-tiktok-beli-tokopedia-rawan-disalahgunakan</t>
-        </is>
-      </c>
-      <c r="E88" t="inlineStr"/>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>Pantas Prabowo Geram! Ada 1.000 Tambang Timah Ilegal di BabelNews5 jam yang lalu</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>Tidak Diketahui</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>https://www.cnbcindonesia.com/news/20250930073414-4-671339/pantas-prabowo-geram-ada-1000-tambang-timah-ilegal-di-babel</t>
-        </is>
-      </c>
-      <c r="E89" t="inlineStr"/>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>InternasionalKemlu Respons Baliho Wajah Presiden Prabowo di Tel Aviv IsraelNews5 jam yang lalu</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>Tidak Diketahui</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>https://www.cnbcindonesia.com/news/20250930081041-4-671351/kemlu-respons-baliho-wajah-presiden-prabowo-di-tel-aviv-israel</t>
-        </is>
-      </c>
-      <c r="E90" t="inlineStr"/>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>Titah Prabowo: TNI-Polri Operasi Besar-Besaran di Babel, Ini AlasannyaNews5 jam yang lalu</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>Tidak Diketahui</t>
-        </is>
-      </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>https://www.cnbcindonesia.com/news/20250930071440-4-671338/titah-prabowo-tni-polri-operasi-besar-besaran-di-babel-ini-alasannya</t>
-        </is>
-      </c>
-      <c r="E91" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>